<commit_message>
added w & w/o tax deduction
</commit_message>
<xml_diff>
--- a/single-calculation.xlsx
+++ b/single-calculation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\4047657\Documents\calculations\hmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62EEE4BA-BE2B-453C-8679-289C913F4CCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC35444-BD8A-4021-BB78-97FE50048D44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60720" yWindow="870" windowWidth="21795" windowHeight="14535" xr2:uid="{61E349DD-C396-4897-954F-94B6F0CC0F58}"/>
   </bookViews>
@@ -19,6 +19,7 @@
     <definedName name="Amount">finance!$B$4</definedName>
     <definedName name="Annual_Rate">finance!$B$1</definedName>
     <definedName name="cap_appreciation_rate">finance!$E$1</definedName>
+    <definedName name="Initial_Value">finance!$B$5</definedName>
     <definedName name="Payments___Year">finance!$B$2</definedName>
     <definedName name="rental_growth">finance!$E$4</definedName>
     <definedName name="rental_income">finance!$E$2</definedName>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>cap_appreciation_rate</t>
   </si>
@@ -99,13 +100,25 @@
     <t>rental growth</t>
   </si>
   <si>
-    <t>cashflow</t>
-  </si>
-  <si>
     <t>net_capital growth</t>
   </si>
   <si>
     <t>cashflow_0</t>
+  </si>
+  <si>
+    <t>Initial Value</t>
+  </si>
+  <si>
+    <t>tax_incentive</t>
+  </si>
+  <si>
+    <t>cashflow (no tax deduction)</t>
+  </si>
+  <si>
+    <t>cashflow (w/ tax deduction)</t>
+  </si>
+  <si>
+    <t>depreciationschedule</t>
   </si>
 </sst>
 </file>
@@ -117,7 +130,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="0.000%"/>
-    <numFmt numFmtId="168" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -177,11 +190,11 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -243,15 +256,160 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>finance!$N$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> cashflow (no tax deduction) </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg2">
+                <a:lumMod val="50000"/>
+                <a:alpha val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="14"/>
+              <c:pt idx="0">
+                <c:v> $1 </c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v> $2 </c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v> $3 </c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v> $4 </c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v> $5 </c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v> $6 </c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v> $7 </c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v> $8 </c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v> $9 </c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v> $10 </c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v> $11 </c:v>
+              </c:pt>
+              <c:pt idx="11">
+                <c:v> $12 </c:v>
+              </c:pt>
+              <c:pt idx="12">
+                <c:v> $13 </c:v>
+              </c:pt>
+              <c:pt idx="13">
+                <c:v> $14 </c:v>
+              </c:pt>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:autoCat val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>finance!$N$28:$N$57</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>finance!$N$28:$N$41</c:f>
+              <c:numCache>
+                <c:formatCode>_-"$"* #,##0_-;\-"$"* #,##0_-;_-"$"* "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>-16237.192575882436</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-14692.792575882435</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-13055.728575882429</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-11320.440735882425</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-9481.0356254824255</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-7531.2662084584226</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-5464.5106264129863</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-3273.7497094448117</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-951.54313745855325</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1509.995828846877</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4119.2271331306401</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6885.0123156714253</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9816.7446091646561</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12924.380840267484</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-85EE-498D-B57F-5F88C9FE5CEF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="6"/>
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>finance!$G$8</c:f>
+              <c:f>finance!$G$27</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> cashflow </c:v>
+                  <c:v> cashflow (w/ tax deduction) </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -274,7 +432,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strLit>
-              <c:ptCount val="15"/>
+              <c:ptCount val="14"/>
               <c:pt idx="0">
                 <c:v> $1 </c:v>
               </c:pt>
@@ -316,9 +474,6 @@
               </c:pt>
               <c:pt idx="13">
                 <c:v> $14 </c:v>
-              </c:pt>
-              <c:pt idx="14">
-                <c:v> $15 </c:v>
               </c:pt>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
@@ -332,58 +487,55 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>finance!$G$9:$G$38</c15:sqref>
+                    <c15:sqref>finance!$G$28:$G$57</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>finance!$G$9:$G$23</c:f>
+              <c:f>finance!$G$28:$G$41</c:f>
               <c:numCache>
                 <c:formatCode>_-"$"* #,##0_-;\-"$"* #,##0_-;_-"$"* "-"??_-;_-@_-</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>-15524.45574502361</c:v>
+                  <c:v>-9507.2005758824362</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-14068.45574502361</c:v>
+                  <c:v>-8055.0663128232127</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-12510.535745023608</c:v>
+                  <c:v>-6515.3795715905026</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-10843.561345023605</c:v>
+                  <c:v>-4882.863690493502</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-9059.8987370236064</c:v>
+                  <c:v>-3151.9241055197335</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-7151.3797464636009</c:v>
+                  <c:v>-1316.6292040305761</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-5109.2644265643976</c:v>
+                  <c:v>629.30997431938704</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-2924.2010342722569</c:v>
+                  <c:v>2692.561258827358</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-586.18320451965701</c:v>
+                  <c:v>4880.1941647151161</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1915.4958733156163</c:v>
+                  <c:v>7199.7040838201901</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4592.29248659937</c:v>
+                  <c:v>9659.0379316886974</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7456.4648628129798</c:v>
+                  <c:v>12266.621338728823</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10521.129305361545</c:v>
+                  <c:v>15031.387478358654</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13800.320258888511</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>17309.054579162352</c:v>
+                  <c:v>17962.807630674055</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -402,9 +554,113 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
+        <c:gapWidth val="150"/>
         <c:axId val="509075144"/>
         <c:axId val="509074424"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="10"/>
+                <c:order val="10"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>finance!$M$27</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>tax_incentive</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>finance!$M$28:$M$57</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>finance!$M$28:$M$41</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
+                      <c:ptCount val="14"/>
+                      <c:pt idx="0">
+                        <c:v>6729.9920000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>6637.7262630592222</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>6540.3490042919266</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>6437.5770453889227</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>6329.111519962692</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>6214.6370044278465</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>6093.8206007323734</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>5966.3109682721697</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>5831.7373021736694</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>5689.7082549733132</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>5539.8107985580573</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>5381.6090230573964</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>5214.6428691939991</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>5038.4267904065691</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-85EE-498D-B57F-5F88C9FE5CEF}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -414,7 +670,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>finance!$H$8</c:f>
+              <c:f>finance!$H$27</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -455,7 +711,7 @@
           </c:marker>
           <c:cat>
             <c:strLit>
-              <c:ptCount val="15"/>
+              <c:ptCount val="14"/>
               <c:pt idx="0">
                 <c:v> $1 </c:v>
               </c:pt>
@@ -497,9 +753,6 @@
               </c:pt>
               <c:pt idx="13">
                 <c:v> $14 </c:v>
-              </c:pt>
-              <c:pt idx="14">
-                <c:v> $15 </c:v>
               </c:pt>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
@@ -513,58 +766,55 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>finance!$H$9:$H$38</c15:sqref>
+                    <c15:sqref>finance!$H$28:$H$57</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>finance!$H$9:$H$23</c:f>
+              <c:f>finance!$H$28:$H$41</c:f>
               <c:numCache>
                 <c:formatCode>_-"$"* #,##0_-;\-"$"* #,##0_-;_-"$"* "-"??_-;_-@_-</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>535000</c:v>
+                  <c:v>795000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>572450</c:v>
+                  <c:v>842700</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>612521.5</c:v>
+                  <c:v>893262</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>655398.005</c:v>
+                  <c:v>946857.72000000009</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>701275.86535000009</c:v>
+                  <c:v>1003669.1832000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>750365.1759245001</c:v>
+                  <c:v>1063889.3341920001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>802890.7382392151</c:v>
+                  <c:v>1127722.6942435203</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>859093.08991596021</c:v>
+                  <c:v>1195386.0558981316</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>919229.60621007753</c:v>
+                  <c:v>1267109.2192520194</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>983575.67864478298</c:v>
+                  <c:v>1343135.7724071406</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1052425.9761499178</c:v>
+                  <c:v>1423723.918751569</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1126095.794480412</c:v>
+                  <c:v>1509147.3538766631</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1204922.500094041</c:v>
+                  <c:v>1599696.1951092631</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1289267.075100624</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1379515.7703576677</c:v>
+                  <c:v>1695677.966815819</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -581,7 +831,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>finance!$I$8</c:f>
+              <c:f>finance!$I$27</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -622,7 +872,7 @@
           </c:marker>
           <c:cat>
             <c:strLit>
-              <c:ptCount val="15"/>
+              <c:ptCount val="14"/>
               <c:pt idx="0">
                 <c:v> $1 </c:v>
               </c:pt>
@@ -664,9 +914,6 @@
               </c:pt>
               <c:pt idx="13">
                 <c:v> $14 </c:v>
-              </c:pt>
-              <c:pt idx="14">
-                <c:v> $15 </c:v>
               </c:pt>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
@@ -680,58 +927,55 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>finance!$I$9:$I$38</c15:sqref>
+                    <c15:sqref>finance!$I$28:$I$57</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>finance!$I$9:$I$23</c:f>
+              <c:f>finance!$I$28:$I$41</c:f>
               <c:numCache>
                 <c:formatCode>_-"$"* #,##0_-;\-"$"* #,##0_-;_-"$"* "-"??_-;_-@_-</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>41324.455745023617</c:v>
+                  <c:v>195927.23257588246</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>85478.378834748641</c:v>
+                  <c:v>252415.79383646883</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>132656.0373098572</c:v>
+                  <c:v>312253.24139089161</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>183065.07029347226</c:v>
+                  <c:v>375638.26873982954</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>236927.41030610428</c:v>
+                  <c:v>442781.36691589851</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>294480.26932299417</c:v>
+                  <c:v>513905.52546164172</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>355977.19298664242</c:v>
+                  <c:v>589246.97508538247</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>421689.18769325677</c:v>
+                  <c:v>669055.97447451542</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>491905.92559903552</c:v>
+                  <c:v>753597.64389341744</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>566937.03294210206</c:v>
+                  <c:v>843152.84834955446</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>647113.46745009965</c:v>
+                  <c:v>938019.1332770749</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>732788.99100362835</c:v>
+                  <c:v>1038511.7158627645</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>824341.74415367399</c:v>
+                  <c:v>1144964.5353252769</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>922175.92954885866</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1026723.61181782</c:v>
+                  <c:v>1257731.3656556825</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -766,7 +1010,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>finance!$A$8</c15:sqref>
+                          <c15:sqref>finance!$A$27</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -807,16 +1051,16 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>finance!$A$9:$A$38</c15:sqref>
+                          <c15:sqref>finance!$A$28:$A$57</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>finance!$A$9:$A$23</c15:sqref>
+                          <c15:sqref>finance!$A$28:$A$41</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="15"/>
+                      <c:ptCount val="14"/>
                       <c:pt idx="0">
                         <c:v>1</c:v>
                       </c:pt>
@@ -858,9 +1102,6 @@
                       </c:pt>
                       <c:pt idx="13">
                         <c:v>14</c:v>
-                      </c:pt>
-                      <c:pt idx="14">
-                        <c:v>15</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -882,7 +1123,7 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>finance!$B$8</c15:sqref>
+                          <c15:sqref>finance!$B$27</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -923,66 +1164,63 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>finance!$B$9:$B$38</c15:sqref>
+                          <c15:sqref>finance!$B$28:$B$57</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>finance!$B$9:$B$23</c15:sqref>
+                          <c15:sqref>finance!$B$28:$B$41</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>#,##0</c:formatCode>
-                      <c:ptCount val="15"/>
+                      <c:ptCount val="14"/>
                       <c:pt idx="0">
-                        <c:v>-36324.45574502361</c:v>
+                        <c:v>-41977.192575882436</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>-36324.45574502361</c:v>
+                        <c:v>-41977.192575882436</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>-36324.45574502361</c:v>
+                        <c:v>-41977.192575882436</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>-36324.45574502361</c:v>
+                        <c:v>-41977.192575882436</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>-36324.45574502361</c:v>
+                        <c:v>-41977.192575882436</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>-36324.45574502361</c:v>
+                        <c:v>-41977.192575882436</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>-36324.45574502361</c:v>
+                        <c:v>-41977.192575882436</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>-36324.45574502361</c:v>
+                        <c:v>-41977.192575882436</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>-36324.45574502361</c:v>
+                        <c:v>-41977.192575882436</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>-36324.45574502361</c:v>
+                        <c:v>-41977.192575882436</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>-36324.45574502361</c:v>
+                        <c:v>-41977.192575882436</c:v>
                       </c:pt>
                       <c:pt idx="11">
-                        <c:v>-36324.45574502361</c:v>
+                        <c:v>-41977.192575882436</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>-36324.45574502361</c:v>
+                        <c:v>-41977.192575882436</c:v>
                       </c:pt>
                       <c:pt idx="13">
-                        <c:v>-36324.45574502361</c:v>
-                      </c:pt>
-                      <c:pt idx="14">
-                        <c:v>-36324.45574502361</c:v>
+                        <c:v>-41977.192575882436</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-1856-4398-A86C-ECCE62D44F1C}"/>
                   </c:ext>
@@ -998,7 +1236,7 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>finance!$C$8</c15:sqref>
+                          <c15:sqref>finance!$C$27</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1039,66 +1277,63 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>finance!$C$9:$C$38</c15:sqref>
+                          <c15:sqref>finance!$C$28:$C$57</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>finance!$C$9:$C$23</c15:sqref>
+                          <c15:sqref>finance!$C$28:$C$41</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>#,##0</c:formatCode>
-                      <c:ptCount val="15"/>
+                      <c:ptCount val="14"/>
                       <c:pt idx="0">
-                        <c:v>-6324.4557450236143</c:v>
+                        <c:v>-8327.2325758824318</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>-6703.9230897250318</c:v>
+                        <c:v>-8788.5612605863171</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>-7106.1584751085329</c:v>
+                        <c:v>-9275.4475544228007</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>-7532.5279836150457</c:v>
+                        <c:v>-9789.3073489378239</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>-7984.4796626319485</c:v>
+                        <c:v>-10331.634976068977</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>-8463.5484423898633</c:v>
+                        <c:v>-10904.007553743199</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>-8971.3613489332565</c:v>
+                        <c:v>-11508.089572220571</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>-9509.6430298692521</c:v>
+                        <c:v>-12145.637734521591</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>-10080.221611661404</c:v>
+                        <c:v>-12818.506065014088</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>-10685.034908361091</c:v>
+                        <c:v>-13528.651301015869</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>-11326.137002862755</c:v>
+                        <c:v>-14278.138583092148</c:v>
                       </c:pt>
                       <c:pt idx="11">
-                        <c:v>-12005.705223034522</c:v>
+                        <c:v>-15069.147460595455</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>-12726.047536416592</c:v>
+                        <c:v>-15903.978229912438</c:v>
                       </c:pt>
                       <c:pt idx="13">
-                        <c:v>-13489.610388601586</c:v>
-                      </c:pt>
-                      <c:pt idx="14">
-                        <c:v>-14298.987011917683</c:v>
+                        <c:v>-16785.058623849593</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-1856-4398-A86C-ECCE62D44F1C}"/>
                   </c:ext>
@@ -1114,7 +1349,7 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>finance!$D$8</c15:sqref>
+                          <c15:sqref>finance!$D$27</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1155,66 +1390,63 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>finance!$D$9:$D$38</c15:sqref>
+                          <c15:sqref>finance!$D$28:$D$57</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>finance!$D$9:$D$23</c15:sqref>
+                          <c15:sqref>finance!$D$28:$D$41</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>#,##0</c:formatCode>
-                      <c:ptCount val="15"/>
+                      <c:ptCount val="14"/>
                       <c:pt idx="0">
-                        <c:v>-30000.000000000004</c:v>
+                        <c:v>-33649.96</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>-29620.532655298583</c:v>
+                        <c:v>-33188.631315296108</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>-29218.297269915078</c:v>
+                        <c:v>-32701.745021459632</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>-28791.927761408566</c:v>
+                        <c:v>-32187.885226944611</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>-28339.976082391666</c:v>
+                        <c:v>-31645.557599813459</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>-27860.90730263375</c:v>
+                        <c:v>-31073.185022139231</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>-27353.094396090357</c:v>
+                        <c:v>-30469.103003661865</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>-26814.812715154363</c:v>
+                        <c:v>-29831.554841360845</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>-26244.23413336221</c:v>
+                        <c:v>-29158.686510868345</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>-25639.420836662524</c:v>
+                        <c:v>-28448.541274866566</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>-24998.318742160856</c:v>
+                        <c:v>-27699.053992790283</c:v>
                       </c:pt>
                       <c:pt idx="11">
-                        <c:v>-24318.750521989092</c:v>
+                        <c:v>-26908.045115286979</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>-23598.408208607023</c:v>
+                        <c:v>-26073.214345969995</c:v>
                       </c:pt>
                       <c:pt idx="13">
-                        <c:v>-22834.845356422033</c:v>
-                      </c:pt>
-                      <c:pt idx="14">
-                        <c:v>-22025.468733105929</c:v>
+                        <c:v>-25192.133952032844</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-1856-4398-A86C-ECCE62D44F1C}"/>
                   </c:ext>
@@ -1230,7 +1462,7 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>finance!$E$8</c15:sqref>
+                          <c15:sqref>finance!$E$27</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1271,66 +1503,63 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>finance!$E$9:$E$38</c15:sqref>
+                          <c15:sqref>finance!$E$28:$E$57</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>finance!$E$9:$E$23</c15:sqref>
+                          <c15:sqref>finance!$E$28:$E$41</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>#,##0</c:formatCode>
-                      <c:ptCount val="15"/>
+                      <c:ptCount val="14"/>
                       <c:pt idx="0">
-                        <c:v>493675.54425497638</c:v>
+                        <c:v>599072.76742411754</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>486971.62116525136</c:v>
+                        <c:v>590284.20616353117</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>479865.4626901428</c:v>
+                        <c:v>581008.75860910839</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>472332.93470652774</c:v>
+                        <c:v>571219.45126017055</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>464348.45504389581</c:v>
+                        <c:v>560887.81628410157</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>455884.90660150594</c:v>
+                        <c:v>549983.80873035837</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>446913.54525257269</c:v>
+                        <c:v>538475.7191581378</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>437403.90222270344</c:v>
+                        <c:v>526330.08142361615</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>427323.68061104201</c:v>
+                        <c:v>513511.57535860204</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>416638.64570268092</c:v>
+                        <c:v>499982.92405758618</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>405312.50869981817</c:v>
+                        <c:v>485704.78547449404</c:v>
                       </c:pt>
                       <c:pt idx="11">
-                        <c:v>393306.80347678362</c:v>
+                        <c:v>470635.63801389857</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>380580.755940367</c:v>
+                        <c:v>454731.65978398611</c:v>
                       </c:pt>
                       <c:pt idx="13">
-                        <c:v>367091.1455517654</c:v>
-                      </c:pt>
-                      <c:pt idx="14">
-                        <c:v>352792.1585398477</c:v>
+                        <c:v>437946.60116013652</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000004-1856-4398-A86C-ECCE62D44F1C}"/>
                   </c:ext>
@@ -1346,7 +1575,7 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>finance!$F$8</c15:sqref>
+                          <c15:sqref>finance!$F$27</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1387,66 +1616,63 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>finance!$F$9:$F$38</c15:sqref>
+                          <c15:sqref>finance!$F$28:$F$57</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>finance!$F$9:$F$23</c15:sqref>
+                          <c15:sqref>finance!$F$28:$F$41</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>#,##0</c:formatCode>
-                      <c:ptCount val="15"/>
+                      <c:ptCount val="14"/>
                       <c:pt idx="0">
-                        <c:v>20800</c:v>
+                        <c:v>25740</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>22256</c:v>
+                        <c:v>27284.400000000001</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>23813.920000000002</c:v>
+                        <c:v>28921.464000000007</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>25480.894400000005</c:v>
+                        <c:v>30656.751840000012</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>27264.557008000003</c:v>
+                        <c:v>32496.156950400011</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>29173.075998560009</c:v>
+                        <c:v>34445.926367424014</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>31215.191318459212</c:v>
+                        <c:v>36512.68194946945</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>33400.254710751353</c:v>
+                        <c:v>38703.442866437625</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>35738.272540503953</c:v>
+                        <c:v>41025.649438423883</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>38239.951618339226</c:v>
+                        <c:v>43487.188404729313</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>40916.74823162298</c:v>
+                        <c:v>46096.419709013076</c:v>
                       </c:pt>
                       <c:pt idx="11">
-                        <c:v>43780.92060783659</c:v>
+                        <c:v>48862.204891553862</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>46845.585050385154</c:v>
+                        <c:v>51793.937185047092</c:v>
                       </c:pt>
                       <c:pt idx="13">
-                        <c:v>50124.77600391212</c:v>
-                      </c:pt>
-                      <c:pt idx="14">
-                        <c:v>53633.510324185962</c:v>
+                        <c:v>54901.57341614992</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-1856-4398-A86C-ECCE62D44F1C}"/>
                   </c:ext>
@@ -1464,7 +1690,7 @@
           <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>finance!$L$8</c:f>
+              <c:f>finance!$L$27</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1487,7 +1713,7 @@
           </c:marker>
           <c:cat>
             <c:strLit>
-              <c:ptCount val="15"/>
+              <c:ptCount val="14"/>
               <c:pt idx="0">
                 <c:v> 1 </c:v>
               </c:pt>
@@ -1529,9 +1755,6 @@
               </c:pt>
               <c:pt idx="13">
                 <c:v> 14 </c:v>
-              </c:pt>
-              <c:pt idx="14">
-                <c:v> 15 </c:v>
               </c:pt>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
@@ -1545,14 +1768,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>finance!$L$9:$L$38</c15:sqref>
+                    <c15:sqref>finance!$L$28:$L$57</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>finance!$L$9:$L$23</c:f>
+              <c:f>finance!$L$28:$L$41</c:f>
               <c:numCache>
                 <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1593,9 +1816,6 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1628,6 +1848,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1784,6 +2005,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="509074424"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -1800,17 +2022,17 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:legendEntry>
-        <c:idx val="3"/>
+        <c:idx val="4"/>
         <c:delete val="1"/>
       </c:legendEntry>
       <c:layout>
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11088057574383105"/>
+          <c:x val="0.1608806401931217"/>
           <c:y val="8.0188066395467564E-2"/>
-          <c:w val="0.25702033738565722"/>
-          <c:h val="0.15532832116877332"/>
+          <c:w val="0.27944186937285614"/>
+          <c:h val="0.24672550962497988"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2433,16 +2655,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>974090</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>53975</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>24765</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>235584</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>60326</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>501649</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>10161</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2468,6 +2690,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2787,10 +3013,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EA2527A-3BE5-4BA5-A375-284826528062}">
-  <dimension ref="A1:Q43"/>
+  <dimension ref="A1:Q62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="Q36" sqref="Q36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2806,26 +3032,28 @@
     <col min="10" max="10" width="11.6640625" customWidth="1"/>
     <col min="11" max="11" width="10.5546875" customWidth="1"/>
     <col min="12" max="12" width="9.5546875" customWidth="1"/>
-    <col min="13" max="16" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="5">
-        <v>0.06</v>
+        <v>5.5399999999999998E-2</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="4">
-        <v>7.0000000000000007E-2</v>
+        <v>0.06</v>
       </c>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -2836,11 +3064,11 @@
         <v>12</v>
       </c>
       <c r="E2" s="7">
-        <v>500</v>
+        <v>660</v>
       </c>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2851,1695 +3079,1951 @@
         <v>14</v>
       </c>
       <c r="E3" s="4">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="2">
-        <v>500000</v>
+        <v>607400</v>
       </c>
       <c r="D4" t="s">
         <v>16</v>
       </c>
       <c r="E4" s="4">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="2">
+        <v>750000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B27" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C27" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D27" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E27" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F27" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G27" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="I27" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="I8" s="12" t="s">
+      <c r="J27" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K27" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="L27" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="J8" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="L8" s="10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9" s="3">
-        <f t="shared" ref="B9:B38" si="0">PMT(Annual_Rate/Payments___Year,Years*Payments___Year,Amount)</f>
-        <v>-36324.45574502361</v>
-      </c>
-      <c r="C9" s="3">
-        <f t="shared" ref="C9:C38" si="1">PPMT(Annual_Rate/Payments___Year,A9,Years*Payments___Year,Amount)</f>
-        <v>-6324.4557450236143</v>
-      </c>
-      <c r="D9" s="3">
-        <f t="shared" ref="D9:D38" si="2">IPMT(Annual_Rate/Payments___Year,A9,Years*Payments___Year,Amount)</f>
-        <v>-30000.000000000004</v>
-      </c>
-      <c r="E9" s="3">
-        <f>Amount+C9</f>
-        <v>493675.54425497638</v>
-      </c>
-      <c r="F9" s="3">
-        <f>52*K9</f>
-        <v>20800</v>
-      </c>
-      <c r="G9" s="8">
-        <f>B9+F9</f>
-        <v>-15524.45574502361</v>
-      </c>
-      <c r="H9" s="8">
-        <f>Amount*(1+cap_appreciation_rate)</f>
-        <v>535000</v>
-      </c>
-      <c r="I9" s="8">
-        <f>H9-E9</f>
-        <v>41324.455745023617</v>
-      </c>
-      <c r="J9" s="1">
-        <f>B9/52</f>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="K9">
-        <f>rental_income*rental_yield</f>
-        <v>400</v>
-      </c>
-      <c r="L9" s="2">
-        <v>0</v>
-      </c>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>2</v>
-      </c>
-      <c r="B10" s="3">
-        <f t="shared" si="0"/>
-        <v>-36324.45574502361</v>
-      </c>
-      <c r="C10" s="3">
-        <f t="shared" si="1"/>
-        <v>-6703.9230897250318</v>
-      </c>
-      <c r="D10" s="3">
-        <f t="shared" si="2"/>
-        <v>-29620.532655298583</v>
-      </c>
-      <c r="E10" s="3">
-        <f>E9+C10</f>
-        <v>486971.62116525136</v>
-      </c>
-      <c r="F10" s="3">
-        <f t="shared" ref="F10:F38" si="3">52*K10</f>
-        <v>22256</v>
-      </c>
-      <c r="G10" s="8">
-        <f>B10+F10</f>
-        <v>-14068.45574502361</v>
-      </c>
-      <c r="H10" s="8">
-        <f>H9*(1+cap_appreciation_rate)</f>
-        <v>572450</v>
-      </c>
-      <c r="I10" s="8">
-        <f t="shared" ref="I10:I38" si="4">H10-E10</f>
-        <v>85478.378834748641</v>
-      </c>
-      <c r="J10" s="1">
-        <f>B10/52</f>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="K10" s="9">
-        <f>K9*(1+rental_growth)</f>
-        <v>428</v>
-      </c>
-      <c r="L10" s="2">
-        <v>0</v>
-      </c>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>3</v>
-      </c>
-      <c r="B11" s="3">
-        <f t="shared" si="0"/>
-        <v>-36324.45574502361</v>
-      </c>
-      <c r="C11" s="3">
-        <f t="shared" si="1"/>
-        <v>-7106.1584751085329</v>
-      </c>
-      <c r="D11" s="3">
-        <f t="shared" si="2"/>
-        <v>-29218.297269915078</v>
-      </c>
-      <c r="E11" s="3">
-        <f t="shared" ref="E11:E38" si="5">E10+C11</f>
-        <v>479865.4626901428</v>
-      </c>
-      <c r="F11" s="3">
-        <f t="shared" si="3"/>
-        <v>23813.920000000002</v>
-      </c>
-      <c r="G11" s="8">
-        <f>B11+F11</f>
-        <v>-12510.535745023608</v>
-      </c>
-      <c r="H11" s="8">
-        <f>H10*(1+cap_appreciation_rate)</f>
-        <v>612521.5</v>
-      </c>
-      <c r="I11" s="8">
-        <f t="shared" si="4"/>
-        <v>132656.0373098572</v>
-      </c>
-      <c r="J11" s="1">
-        <f>B11/52</f>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="K11" s="9">
-        <f>K10*(1+rental_growth)</f>
-        <v>457.96000000000004</v>
-      </c>
-      <c r="L11" s="2">
-        <v>0</v>
-      </c>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>4</v>
-      </c>
-      <c r="B12" s="3">
-        <f t="shared" si="0"/>
-        <v>-36324.45574502361</v>
-      </c>
-      <c r="C12" s="3">
-        <f t="shared" si="1"/>
-        <v>-7532.5279836150457</v>
-      </c>
-      <c r="D12" s="3">
-        <f t="shared" si="2"/>
-        <v>-28791.927761408566</v>
-      </c>
-      <c r="E12" s="3">
-        <f t="shared" si="5"/>
-        <v>472332.93470652774</v>
-      </c>
-      <c r="F12" s="3">
-        <f t="shared" si="3"/>
-        <v>25480.894400000005</v>
-      </c>
-      <c r="G12" s="8">
-        <f>B12+F12</f>
-        <v>-10843.561345023605</v>
-      </c>
-      <c r="H12" s="8">
-        <f>H11*(1+cap_appreciation_rate)</f>
-        <v>655398.005</v>
-      </c>
-      <c r="I12" s="8">
-        <f t="shared" si="4"/>
-        <v>183065.07029347226</v>
-      </c>
-      <c r="J12" s="1">
-        <f>B12/52</f>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="K12" s="9">
-        <f>K11*(1+rental_growth)</f>
-        <v>490.01720000000006</v>
-      </c>
-      <c r="L12" s="2">
-        <v>0</v>
-      </c>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>5</v>
-      </c>
-      <c r="B13" s="3">
-        <f t="shared" si="0"/>
-        <v>-36324.45574502361</v>
-      </c>
-      <c r="C13" s="3">
-        <f t="shared" si="1"/>
-        <v>-7984.4796626319485</v>
-      </c>
-      <c r="D13" s="3">
-        <f t="shared" si="2"/>
-        <v>-28339.976082391666</v>
-      </c>
-      <c r="E13" s="3">
-        <f t="shared" si="5"/>
-        <v>464348.45504389581</v>
-      </c>
-      <c r="F13" s="3">
-        <f t="shared" si="3"/>
-        <v>27264.557008000003</v>
-      </c>
-      <c r="G13" s="8">
-        <f>B13+F13</f>
-        <v>-9059.8987370236064</v>
-      </c>
-      <c r="H13" s="8">
-        <f>H12*(1+cap_appreciation_rate)</f>
-        <v>701275.86535000009</v>
-      </c>
-      <c r="I13" s="8">
-        <f t="shared" si="4"/>
-        <v>236927.41030610428</v>
-      </c>
-      <c r="J13" s="1">
-        <f>B13/52</f>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="K13" s="9">
-        <f>K12*(1+rental_growth)</f>
-        <v>524.3184040000001</v>
-      </c>
-      <c r="L13" s="2">
-        <v>0</v>
-      </c>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>6</v>
-      </c>
-      <c r="B14" s="3">
-        <f t="shared" si="0"/>
-        <v>-36324.45574502361</v>
-      </c>
-      <c r="C14" s="3">
-        <f t="shared" si="1"/>
-        <v>-8463.5484423898633</v>
-      </c>
-      <c r="D14" s="3">
-        <f t="shared" si="2"/>
-        <v>-27860.90730263375</v>
-      </c>
-      <c r="E14" s="3">
-        <f t="shared" si="5"/>
-        <v>455884.90660150594</v>
-      </c>
-      <c r="F14" s="3">
-        <f t="shared" si="3"/>
-        <v>29173.075998560009</v>
-      </c>
-      <c r="G14" s="8">
-        <f>B14+F14</f>
-        <v>-7151.3797464636009</v>
-      </c>
-      <c r="H14" s="8">
-        <f>H13*(1+cap_appreciation_rate)</f>
-        <v>750365.1759245001</v>
-      </c>
-      <c r="I14" s="8">
-        <f t="shared" si="4"/>
-        <v>294480.26932299417</v>
-      </c>
-      <c r="J14" s="1">
-        <f>B14/52</f>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="K14" s="9">
-        <f>K13*(1+rental_growth)</f>
-        <v>561.02069228000016</v>
-      </c>
-      <c r="L14" s="2">
-        <v>0</v>
-      </c>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="2"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>7</v>
-      </c>
-      <c r="B15" s="3">
-        <f t="shared" si="0"/>
-        <v>-36324.45574502361</v>
-      </c>
-      <c r="C15" s="3">
-        <f t="shared" si="1"/>
-        <v>-8971.3613489332565</v>
-      </c>
-      <c r="D15" s="3">
-        <f t="shared" si="2"/>
-        <v>-27353.094396090357</v>
-      </c>
-      <c r="E15" s="3">
-        <f t="shared" si="5"/>
-        <v>446913.54525257269</v>
-      </c>
-      <c r="F15" s="3">
-        <f t="shared" si="3"/>
-        <v>31215.191318459212</v>
-      </c>
-      <c r="G15" s="8">
-        <f>B15+F15</f>
-        <v>-5109.2644265643976</v>
-      </c>
-      <c r="H15" s="8">
-        <f>H14*(1+cap_appreciation_rate)</f>
-        <v>802890.7382392151</v>
-      </c>
-      <c r="I15" s="8">
-        <f t="shared" si="4"/>
-        <v>355977.19298664242</v>
-      </c>
-      <c r="J15" s="1">
-        <f>B15/52</f>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="K15" s="9">
-        <f>K14*(1+rental_growth)</f>
-        <v>600.2921407396002</v>
-      </c>
-      <c r="L15" s="2">
-        <v>0</v>
-      </c>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>8</v>
-      </c>
-      <c r="B16" s="3">
-        <f t="shared" si="0"/>
-        <v>-36324.45574502361</v>
-      </c>
-      <c r="C16" s="3">
-        <f t="shared" si="1"/>
-        <v>-9509.6430298692521</v>
-      </c>
-      <c r="D16" s="3">
-        <f t="shared" si="2"/>
-        <v>-26814.812715154363</v>
-      </c>
-      <c r="E16" s="3">
-        <f t="shared" si="5"/>
-        <v>437403.90222270344</v>
-      </c>
-      <c r="F16" s="3">
-        <f t="shared" si="3"/>
-        <v>33400.254710751353</v>
-      </c>
-      <c r="G16" s="8">
-        <f>B16+F16</f>
-        <v>-2924.2010342722569</v>
-      </c>
-      <c r="H16" s="8">
-        <f>H15*(1+cap_appreciation_rate)</f>
-        <v>859093.08991596021</v>
-      </c>
-      <c r="I16" s="8">
-        <f t="shared" si="4"/>
-        <v>421689.18769325677</v>
-      </c>
-      <c r="J16" s="1">
-        <f>B16/52</f>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="K16" s="9">
-        <f>K15*(1+rental_growth)</f>
-        <v>642.31259059137221</v>
-      </c>
-      <c r="L16" s="2">
-        <v>0</v>
-      </c>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="2"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>9</v>
-      </c>
-      <c r="B17" s="3">
-        <f t="shared" si="0"/>
-        <v>-36324.45574502361</v>
-      </c>
-      <c r="C17" s="3">
-        <f t="shared" si="1"/>
-        <v>-10080.221611661404</v>
-      </c>
-      <c r="D17" s="3">
-        <f t="shared" si="2"/>
-        <v>-26244.23413336221</v>
-      </c>
-      <c r="E17" s="3">
-        <f t="shared" si="5"/>
-        <v>427323.68061104201</v>
-      </c>
-      <c r="F17" s="3">
-        <f t="shared" si="3"/>
-        <v>35738.272540503953</v>
-      </c>
-      <c r="G17" s="8">
-        <f>B17+F17</f>
-        <v>-586.18320451965701</v>
-      </c>
-      <c r="H17" s="8">
-        <f>H16*(1+cap_appreciation_rate)</f>
-        <v>919229.60621007753</v>
-      </c>
-      <c r="I17" s="8">
-        <f t="shared" si="4"/>
-        <v>491905.92559903552</v>
-      </c>
-      <c r="J17" s="1">
-        <f>B17/52</f>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="K17" s="9">
-        <f>K16*(1+rental_growth)</f>
-        <v>687.27447193276828</v>
-      </c>
-      <c r="L17" s="2">
-        <v>0</v>
-      </c>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
-      <c r="Q17" s="2"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>10</v>
-      </c>
-      <c r="B18" s="3">
-        <f t="shared" si="0"/>
-        <v>-36324.45574502361</v>
-      </c>
-      <c r="C18" s="3">
-        <f t="shared" si="1"/>
-        <v>-10685.034908361091</v>
-      </c>
-      <c r="D18" s="3">
-        <f t="shared" si="2"/>
-        <v>-25639.420836662524</v>
-      </c>
-      <c r="E18" s="3">
-        <f t="shared" si="5"/>
-        <v>416638.64570268092</v>
-      </c>
-      <c r="F18" s="3">
-        <f t="shared" si="3"/>
-        <v>38239.951618339226</v>
-      </c>
-      <c r="G18" s="8">
-        <f>B18+F18</f>
-        <v>1915.4958733156163</v>
-      </c>
-      <c r="H18" s="8">
-        <f>H17*(1+cap_appreciation_rate)</f>
-        <v>983575.67864478298</v>
-      </c>
-      <c r="I18" s="8">
-        <f t="shared" si="4"/>
-        <v>566937.03294210206</v>
-      </c>
-      <c r="J18" s="1">
-        <f>B18/52</f>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="K18" s="9">
-        <f>K17*(1+rental_growth)</f>
-        <v>735.38368496806208</v>
-      </c>
-      <c r="L18" s="2">
-        <v>0</v>
-      </c>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
-      <c r="Q18" s="2"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>11</v>
-      </c>
-      <c r="B19" s="3">
-        <f t="shared" si="0"/>
-        <v>-36324.45574502361</v>
-      </c>
-      <c r="C19" s="3">
-        <f t="shared" si="1"/>
-        <v>-11326.137002862755</v>
-      </c>
-      <c r="D19" s="3">
-        <f t="shared" si="2"/>
-        <v>-24998.318742160856</v>
-      </c>
-      <c r="E19" s="3">
-        <f t="shared" si="5"/>
-        <v>405312.50869981817</v>
-      </c>
-      <c r="F19" s="3">
-        <f t="shared" si="3"/>
-        <v>40916.74823162298</v>
-      </c>
-      <c r="G19" s="8">
-        <f>B19+F19</f>
-        <v>4592.29248659937</v>
-      </c>
-      <c r="H19" s="8">
-        <f>H18*(1+cap_appreciation_rate)</f>
-        <v>1052425.9761499178</v>
-      </c>
-      <c r="I19" s="8">
-        <f t="shared" si="4"/>
-        <v>647113.46745009965</v>
-      </c>
-      <c r="J19" s="1">
-        <f>B19/52</f>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="K19" s="9">
-        <f>K18*(1+rental_growth)</f>
-        <v>786.8605429158265</v>
-      </c>
-      <c r="L19" s="2">
-        <v>0</v>
-      </c>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
-      <c r="Q19" s="2"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>12</v>
-      </c>
-      <c r="B20" s="3">
-        <f t="shared" si="0"/>
-        <v>-36324.45574502361</v>
-      </c>
-      <c r="C20" s="3">
-        <f t="shared" si="1"/>
-        <v>-12005.705223034522</v>
-      </c>
-      <c r="D20" s="3">
-        <f t="shared" si="2"/>
-        <v>-24318.750521989092</v>
-      </c>
-      <c r="E20" s="3">
-        <f t="shared" si="5"/>
-        <v>393306.80347678362</v>
-      </c>
-      <c r="F20" s="3">
-        <f t="shared" si="3"/>
-        <v>43780.92060783659</v>
-      </c>
-      <c r="G20" s="8">
-        <f>B20+F20</f>
-        <v>7456.4648628129798</v>
-      </c>
-      <c r="H20" s="8">
-        <f>H19*(1+cap_appreciation_rate)</f>
-        <v>1126095.794480412</v>
-      </c>
-      <c r="I20" s="8">
-        <f t="shared" si="4"/>
-        <v>732788.99100362835</v>
-      </c>
-      <c r="J20" s="1">
-        <f>B20/52</f>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="K20" s="9">
-        <f>K19*(1+rental_growth)</f>
-        <v>841.94078091993435</v>
-      </c>
-      <c r="L20" s="2">
-        <v>0</v>
-      </c>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
-      <c r="Q20" s="2"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>13</v>
-      </c>
-      <c r="B21" s="3">
-        <f t="shared" si="0"/>
-        <v>-36324.45574502361</v>
-      </c>
-      <c r="C21" s="3">
-        <f t="shared" si="1"/>
-        <v>-12726.047536416592</v>
-      </c>
-      <c r="D21" s="3">
-        <f t="shared" si="2"/>
-        <v>-23598.408208607023</v>
-      </c>
-      <c r="E21" s="3">
-        <f t="shared" si="5"/>
-        <v>380580.755940367</v>
-      </c>
-      <c r="F21" s="3">
-        <f t="shared" si="3"/>
-        <v>46845.585050385154</v>
-      </c>
-      <c r="G21" s="8">
-        <f>B21+F21</f>
-        <v>10521.129305361545</v>
-      </c>
-      <c r="H21" s="8">
-        <f>H20*(1+cap_appreciation_rate)</f>
-        <v>1204922.500094041</v>
-      </c>
-      <c r="I21" s="8">
-        <f t="shared" si="4"/>
-        <v>824341.74415367399</v>
-      </c>
-      <c r="J21" s="1">
-        <f>B21/52</f>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="K21" s="9">
-        <f>K20*(1+rental_growth)</f>
-        <v>900.87663558432985</v>
-      </c>
-      <c r="L21" s="2">
-        <v>0</v>
-      </c>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
-      <c r="P21" s="2"/>
-      <c r="Q21" s="2"/>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>14</v>
-      </c>
-      <c r="B22" s="3">
-        <f t="shared" si="0"/>
-        <v>-36324.45574502361</v>
-      </c>
-      <c r="C22" s="3">
-        <f t="shared" si="1"/>
-        <v>-13489.610388601586</v>
-      </c>
-      <c r="D22" s="3">
-        <f t="shared" si="2"/>
-        <v>-22834.845356422033</v>
-      </c>
-      <c r="E22" s="3">
-        <f t="shared" si="5"/>
-        <v>367091.1455517654</v>
-      </c>
-      <c r="F22" s="3">
-        <f t="shared" si="3"/>
-        <v>50124.77600391212</v>
-      </c>
-      <c r="G22" s="8">
-        <f>B22+F22</f>
-        <v>13800.320258888511</v>
-      </c>
-      <c r="H22" s="8">
-        <f>H21*(1+cap_appreciation_rate)</f>
-        <v>1289267.075100624</v>
-      </c>
-      <c r="I22" s="8">
-        <f t="shared" si="4"/>
-        <v>922175.92954885866</v>
-      </c>
-      <c r="J22" s="1">
-        <f>B22/52</f>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="K22" s="9">
-        <f>K21*(1+rental_growth)</f>
-        <v>963.93800007523305</v>
-      </c>
-      <c r="L22" s="2">
-        <v>0</v>
-      </c>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-      <c r="O22" s="2"/>
-      <c r="P22" s="2"/>
-      <c r="Q22" s="2"/>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>15</v>
-      </c>
-      <c r="B23" s="3">
-        <f t="shared" si="0"/>
-        <v>-36324.45574502361</v>
-      </c>
-      <c r="C23" s="3">
-        <f t="shared" si="1"/>
-        <v>-14298.987011917683</v>
-      </c>
-      <c r="D23" s="3">
-        <f t="shared" si="2"/>
-        <v>-22025.468733105929</v>
-      </c>
-      <c r="E23" s="3">
-        <f t="shared" si="5"/>
-        <v>352792.1585398477</v>
-      </c>
-      <c r="F23" s="3">
-        <f t="shared" si="3"/>
-        <v>53633.510324185962</v>
-      </c>
-      <c r="G23" s="8">
-        <f>B23+F23</f>
-        <v>17309.054579162352</v>
-      </c>
-      <c r="H23" s="8">
-        <f>H22*(1+cap_appreciation_rate)</f>
-        <v>1379515.7703576677</v>
-      </c>
-      <c r="I23" s="8">
-        <f t="shared" si="4"/>
-        <v>1026723.61181782</v>
-      </c>
-      <c r="J23" s="1">
-        <f>B23/52</f>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="K23" s="9">
-        <f>K22*(1+rental_growth)</f>
-        <v>1031.4136600804993</v>
-      </c>
-      <c r="L23" s="2">
-        <v>0</v>
-      </c>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-      <c r="O23" s="2"/>
-      <c r="P23" s="2"/>
-      <c r="Q23" s="2"/>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>16</v>
-      </c>
-      <c r="B24" s="3">
-        <f t="shared" si="0"/>
-        <v>-36324.45574502361</v>
-      </c>
-      <c r="C24" s="3">
-        <f t="shared" si="1"/>
-        <v>-15156.926232632744</v>
-      </c>
-      <c r="D24" s="3">
-        <f t="shared" si="2"/>
-        <v>-21167.529512390873</v>
-      </c>
-      <c r="E24" s="3">
-        <f t="shared" si="5"/>
-        <v>337635.23230721499</v>
-      </c>
-      <c r="F24" s="3">
-        <f t="shared" si="3"/>
-        <v>57387.856046878987</v>
-      </c>
-      <c r="G24" s="8">
-        <f>B24+F24</f>
-        <v>21063.400301855378</v>
-      </c>
-      <c r="H24" s="8">
-        <f>H23*(1+cap_appreciation_rate)</f>
-        <v>1476081.8742827044</v>
-      </c>
-      <c r="I24" s="8">
-        <f t="shared" si="4"/>
-        <v>1138446.6419754894</v>
-      </c>
-      <c r="J24" s="1">
-        <f>B24/52</f>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="K24" s="9">
-        <f>K23*(1+rental_growth)</f>
-        <v>1103.6126162861344</v>
-      </c>
-      <c r="L24" s="2">
-        <v>0</v>
-      </c>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
-      <c r="O24" s="2"/>
-      <c r="P24" s="2"/>
-      <c r="Q24" s="2"/>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>17</v>
-      </c>
-      <c r="B25" s="3">
-        <f t="shared" si="0"/>
-        <v>-36324.45574502361</v>
-      </c>
-      <c r="C25" s="3">
-        <f t="shared" si="1"/>
-        <v>-16066.341806590708</v>
-      </c>
-      <c r="D25" s="3">
-        <f t="shared" si="2"/>
-        <v>-20258.113938432904</v>
-      </c>
-      <c r="E25" s="3">
-        <f t="shared" si="5"/>
-        <v>321568.89050062426</v>
-      </c>
-      <c r="F25" s="3">
-        <f t="shared" si="3"/>
-        <v>61405.005970160528</v>
-      </c>
-      <c r="G25" s="8">
-        <f>B25+F25</f>
-        <v>25080.550225136918</v>
-      </c>
-      <c r="H25" s="8">
-        <f>H24*(1+cap_appreciation_rate)</f>
-        <v>1579407.6054824938</v>
-      </c>
-      <c r="I25" s="8">
-        <f t="shared" si="4"/>
-        <v>1257838.7149818696</v>
-      </c>
-      <c r="J25" s="1">
-        <f>B25/52</f>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="K25" s="9">
-        <f>K24*(1+rental_growth)</f>
-        <v>1180.865499426164</v>
-      </c>
-      <c r="L25" s="2">
-        <v>0</v>
-      </c>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
-      <c r="O25" s="2"/>
-      <c r="P25" s="2"/>
-      <c r="Q25" s="2"/>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>18</v>
-      </c>
-      <c r="B26" s="3">
-        <f t="shared" si="0"/>
-        <v>-36324.45574502361</v>
-      </c>
-      <c r="C26" s="3">
-        <f t="shared" si="1"/>
-        <v>-17030.322314986151</v>
-      </c>
-      <c r="D26" s="3">
-        <f t="shared" si="2"/>
-        <v>-19294.133430037466</v>
-      </c>
-      <c r="E26" s="3">
-        <f t="shared" si="5"/>
-        <v>304538.56818563811</v>
-      </c>
-      <c r="F26" s="3">
-        <f t="shared" si="3"/>
-        <v>65703.35638807177</v>
-      </c>
-      <c r="G26" s="8">
-        <f>B26+F26</f>
-        <v>29378.90064304816</v>
-      </c>
-      <c r="H26" s="8">
-        <f>H25*(1+cap_appreciation_rate)</f>
-        <v>1689966.1378662684</v>
-      </c>
-      <c r="I26" s="8">
-        <f t="shared" si="4"/>
-        <v>1385427.5696806302</v>
-      </c>
-      <c r="J26" s="1">
-        <f>B26/52</f>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="K26" s="9">
-        <f>K25*(1+rental_growth)</f>
-        <v>1263.5260843859955</v>
-      </c>
-      <c r="L26" s="2">
-        <v>0</v>
-      </c>
-      <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
-      <c r="O26" s="2"/>
-      <c r="P26" s="2"/>
-      <c r="Q26" s="2"/>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>19</v>
-      </c>
-      <c r="B27" s="3">
-        <f t="shared" si="0"/>
-        <v>-36324.45574502361</v>
-      </c>
-      <c r="C27" s="3">
-        <f t="shared" si="1"/>
-        <v>-18052.141653885319</v>
-      </c>
-      <c r="D27" s="3">
-        <f t="shared" si="2"/>
-        <v>-18272.314091138294</v>
-      </c>
-      <c r="E27" s="3">
-        <f t="shared" si="5"/>
-        <v>286486.4265317528</v>
-      </c>
-      <c r="F27" s="3">
-        <f t="shared" si="3"/>
-        <v>70302.591335236793</v>
-      </c>
-      <c r="G27" s="8">
-        <f>B27+F27</f>
-        <v>33978.135590213184</v>
-      </c>
-      <c r="H27" s="8">
-        <f>H26*(1+cap_appreciation_rate)</f>
-        <v>1808263.7675169073</v>
-      </c>
-      <c r="I27" s="8">
-        <f t="shared" si="4"/>
-        <v>1521777.3409851545</v>
-      </c>
-      <c r="J27" s="1">
-        <f>B27/52</f>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="K27" s="9">
-        <f>K26*(1+rental_growth)</f>
-        <v>1351.9729102930153</v>
-      </c>
-      <c r="L27" s="2">
-        <v>0</v>
-      </c>
-      <c r="M27" s="2"/>
-      <c r="N27" s="2"/>
-      <c r="O27" s="2"/>
-      <c r="P27" s="2"/>
-      <c r="Q27" s="2"/>
+      <c r="M27" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="N27" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="O27" s="10" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="B28" s="3">
-        <f t="shared" si="0"/>
-        <v>-36324.45574502361</v>
+        <f t="shared" ref="B28:B57" si="0">PMT(Annual_Rate/Payments___Year,Years*Payments___Year,Amount)</f>
+        <v>-41977.192575882436</v>
       </c>
       <c r="C28" s="3">
-        <f t="shared" si="1"/>
-        <v>-19135.270153118439</v>
+        <f t="shared" ref="C28:C57" si="1">PPMT(Annual_Rate/Payments___Year,A28,Years*Payments___Year,Amount)</f>
+        <v>-8327.2325758824318</v>
       </c>
       <c r="D28" s="3">
-        <f t="shared" si="2"/>
-        <v>-17189.185591905174</v>
+        <f t="shared" ref="D28:D57" si="2">IPMT(Annual_Rate/Payments___Year,A28,Years*Payments___Year,Amount)</f>
+        <v>-33649.96</v>
       </c>
       <c r="E28" s="3">
-        <f t="shared" si="5"/>
-        <v>267351.15637863439</v>
+        <f>Amount+C28</f>
+        <v>599072.76742411754</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" si="3"/>
-        <v>75223.772728703378</v>
+        <f>52*K28</f>
+        <v>25740</v>
       </c>
       <c r="G28" s="8">
-        <f>B28+F28</f>
-        <v>38899.316983679768</v>
+        <f>B28+F28+M28</f>
+        <v>-9507.2005758824362</v>
       </c>
       <c r="H28" s="8">
-        <f>H27*(1+cap_appreciation_rate)</f>
-        <v>1934842.2312430909</v>
+        <f>Initial_Value*(1+cap_appreciation_rate)</f>
+        <v>795000</v>
       </c>
       <c r="I28" s="8">
-        <f t="shared" si="4"/>
-        <v>1667491.0748644564</v>
+        <f>H28-E28</f>
+        <v>195927.23257588246</v>
       </c>
       <c r="J28" s="1">
-        <f>B28/52</f>
-        <v>-698.54722586583864</v>
-      </c>
-      <c r="K28" s="9">
-        <f>K27*(1+rental_growth)</f>
-        <v>1446.6110140135265</v>
+        <f t="shared" ref="J28:J57" si="3">B28/52</f>
+        <v>-807.2537033823545</v>
+      </c>
+      <c r="K28">
+        <f>rental_income*rental_yield</f>
+        <v>495</v>
       </c>
       <c r="L28" s="2">
         <v>0</v>
       </c>
-      <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
+      <c r="M28" s="2">
+        <f>-D28*0.2</f>
+        <v>6729.9920000000002</v>
+      </c>
+      <c r="N28" s="8">
+        <f>B28+F28</f>
+        <v>-16237.192575882436</v>
+      </c>
       <c r="O28" s="2"/>
       <c r="P28" s="2"/>
       <c r="Q28" s="2"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="B29" s="3">
         <f t="shared" si="0"/>
-        <v>-36324.45574502361</v>
+        <v>-41977.192575882436</v>
       </c>
       <c r="C29" s="3">
         <f t="shared" si="1"/>
-        <v>-20283.386362305544</v>
+        <v>-8788.5612605863171</v>
       </c>
       <c r="D29" s="3">
         <f t="shared" si="2"/>
-        <v>-16041.069382718066</v>
+        <v>-33188.631315296108</v>
       </c>
       <c r="E29" s="3">
-        <f t="shared" si="5"/>
-        <v>247067.77001632884</v>
+        <f>E28+C29</f>
+        <v>590284.20616353117</v>
       </c>
       <c r="F29" s="3">
+        <f t="shared" ref="F29:F57" si="4">52*K29</f>
+        <v>27284.400000000001</v>
+      </c>
+      <c r="G29" s="8">
+        <f t="shared" ref="G29:G57" si="5">B29+F29+M29</f>
+        <v>-8055.0663128232127</v>
+      </c>
+      <c r="H29" s="8">
+        <f t="shared" ref="H29:H57" si="6">H28*(1+cap_appreciation_rate)</f>
+        <v>842700</v>
+      </c>
+      <c r="I29" s="8">
+        <f t="shared" ref="I29:I57" si="7">H29-E29</f>
+        <v>252415.79383646883</v>
+      </c>
+      <c r="J29" s="1">
         <f t="shared" si="3"/>
-        <v>80489.436819712617</v>
-      </c>
-      <c r="G29" s="8">
-        <f>B29+F29</f>
-        <v>44164.981074689007</v>
-      </c>
-      <c r="H29" s="8">
-        <f>H28*(1+cap_appreciation_rate)</f>
-        <v>2070281.1874301075</v>
-      </c>
-      <c r="I29" s="8">
-        <f t="shared" si="4"/>
-        <v>1823213.4174137786</v>
-      </c>
-      <c r="J29" s="1">
-        <f>B29/52</f>
-        <v>-698.54722586583864</v>
+        <v>-807.2537033823545</v>
       </c>
       <c r="K29" s="9">
-        <f>K28*(1+rental_growth)</f>
-        <v>1547.8737849944735</v>
+        <f t="shared" ref="K29:K57" si="8">K28*(1+rental_growth)</f>
+        <v>524.70000000000005</v>
       </c>
       <c r="L29" s="2">
         <v>0</v>
       </c>
-      <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
+      <c r="M29" s="2">
+        <f t="shared" ref="M29:M57" si="9">-D29*0.2</f>
+        <v>6637.7262630592222</v>
+      </c>
+      <c r="N29" s="8">
+        <f t="shared" ref="N29:N57" si="10">B29+F29</f>
+        <v>-14692.792575882435</v>
+      </c>
       <c r="O29" s="2"/>
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="B30" s="3">
         <f t="shared" si="0"/>
-        <v>-36324.45574502361</v>
+        <v>-41977.192575882436</v>
       </c>
       <c r="C30" s="3">
         <f t="shared" si="1"/>
-        <v>-21500.389544043876</v>
+        <v>-9275.4475544228007</v>
       </c>
       <c r="D30" s="3">
         <f t="shared" si="2"/>
-        <v>-14824.066200979736</v>
+        <v>-32701.745021459632</v>
       </c>
       <c r="E30" s="3">
+        <f t="shared" ref="E30:E57" si="11">E29+C30</f>
+        <v>581008.75860910839</v>
+      </c>
+      <c r="F30" s="3">
+        <f t="shared" si="4"/>
+        <v>28921.464000000007</v>
+      </c>
+      <c r="G30" s="8">
         <f t="shared" si="5"/>
-        <v>225567.38047228497</v>
-      </c>
-      <c r="F30" s="3">
+        <v>-6515.3795715905026</v>
+      </c>
+      <c r="H30" s="8">
+        <f t="shared" si="6"/>
+        <v>893262</v>
+      </c>
+      <c r="I30" s="8">
+        <f t="shared" si="7"/>
+        <v>312253.24139089161</v>
+      </c>
+      <c r="J30" s="1">
         <f t="shared" si="3"/>
-        <v>86123.697397092517</v>
-      </c>
-      <c r="G30" s="8">
-        <f>B30+F30</f>
-        <v>49799.241652068908</v>
-      </c>
-      <c r="H30" s="8">
-        <f>H29*(1+cap_appreciation_rate)</f>
-        <v>2215200.8705502152</v>
-      </c>
-      <c r="I30" s="8">
-        <f t="shared" si="4"/>
-        <v>1989633.4900779303</v>
-      </c>
-      <c r="J30" s="1">
-        <f>B30/52</f>
-        <v>-698.54722586583864</v>
+        <v>-807.2537033823545</v>
       </c>
       <c r="K30" s="9">
-        <f>K29*(1+rental_growth)</f>
-        <v>1656.2249499440868</v>
+        <f t="shared" si="8"/>
+        <v>556.18200000000013</v>
       </c>
       <c r="L30" s="2">
         <v>0</v>
       </c>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
+      <c r="M30" s="2">
+        <f t="shared" si="9"/>
+        <v>6540.3490042919266</v>
+      </c>
+      <c r="N30" s="8">
+        <f t="shared" si="10"/>
+        <v>-13055.728575882429</v>
+      </c>
       <c r="O30" s="2"/>
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="B31" s="3">
         <f t="shared" si="0"/>
-        <v>-36324.45574502361</v>
+        <v>-41977.192575882436</v>
       </c>
       <c r="C31" s="3">
         <f t="shared" si="1"/>
-        <v>-22790.41291668651</v>
+        <v>-9789.3073489378239</v>
       </c>
       <c r="D31" s="3">
         <f t="shared" si="2"/>
-        <v>-13534.042828337102</v>
+        <v>-32187.885226944611</v>
       </c>
       <c r="E31" s="3">
+        <f t="shared" si="11"/>
+        <v>571219.45126017055</v>
+      </c>
+      <c r="F31" s="3">
+        <f t="shared" si="4"/>
+        <v>30656.751840000012</v>
+      </c>
+      <c r="G31" s="8">
         <f t="shared" si="5"/>
-        <v>202776.96755559847</v>
-      </c>
-      <c r="F31" s="3">
+        <v>-4882.863690493502</v>
+      </c>
+      <c r="H31" s="8">
+        <f t="shared" si="6"/>
+        <v>946857.72000000009</v>
+      </c>
+      <c r="I31" s="8">
+        <f t="shared" si="7"/>
+        <v>375638.26873982954</v>
+      </c>
+      <c r="J31" s="1">
         <f t="shared" si="3"/>
-        <v>92152.356214889005</v>
-      </c>
-      <c r="G31" s="8">
-        <f>B31+F31</f>
-        <v>55827.900469865395</v>
-      </c>
-      <c r="H31" s="8">
-        <f>H30*(1+cap_appreciation_rate)</f>
-        <v>2370264.9314887305</v>
-      </c>
-      <c r="I31" s="8">
-        <f t="shared" si="4"/>
-        <v>2167487.9639331321</v>
-      </c>
-      <c r="J31" s="1">
-        <f>B31/52</f>
-        <v>-698.54722586583864</v>
+        <v>-807.2537033823545</v>
       </c>
       <c r="K31" s="9">
-        <f>K30*(1+rental_growth)</f>
-        <v>1772.1606964401731</v>
+        <f t="shared" si="8"/>
+        <v>589.5529200000002</v>
       </c>
       <c r="L31" s="2">
         <v>0</v>
       </c>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
+      <c r="M31" s="2">
+        <f t="shared" si="9"/>
+        <v>6437.5770453889227</v>
+      </c>
+      <c r="N31" s="8">
+        <f t="shared" si="10"/>
+        <v>-11320.440735882425</v>
+      </c>
       <c r="O31" s="2"/>
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="B32" s="3">
         <f t="shared" si="0"/>
-        <v>-36324.45574502361</v>
+        <v>-41977.192575882436</v>
       </c>
       <c r="C32" s="3">
         <f t="shared" si="1"/>
-        <v>-24157.837691687702</v>
+        <v>-10331.634976068977</v>
       </c>
       <c r="D32" s="3">
         <f t="shared" si="2"/>
-        <v>-12166.618053335913</v>
+        <v>-31645.557599813459</v>
       </c>
       <c r="E32" s="3">
+        <f t="shared" si="11"/>
+        <v>560887.81628410157</v>
+      </c>
+      <c r="F32" s="3">
+        <f t="shared" si="4"/>
+        <v>32496.156950400011</v>
+      </c>
+      <c r="G32" s="8">
         <f t="shared" si="5"/>
-        <v>178619.12986391078</v>
-      </c>
-      <c r="F32" s="3">
+        <v>-3151.9241055197335</v>
+      </c>
+      <c r="H32" s="8">
+        <f t="shared" si="6"/>
+        <v>1003669.1832000001</v>
+      </c>
+      <c r="I32" s="8">
+        <f t="shared" si="7"/>
+        <v>442781.36691589851</v>
+      </c>
+      <c r="J32" s="1">
         <f t="shared" si="3"/>
-        <v>98603.021149931228</v>
-      </c>
-      <c r="G32" s="8">
-        <f>B32+F32</f>
-        <v>62278.565404907618</v>
-      </c>
-      <c r="H32" s="8">
-        <f>H31*(1+cap_appreciation_rate)</f>
-        <v>2536183.476692942</v>
-      </c>
-      <c r="I32" s="8">
-        <f t="shared" si="4"/>
-        <v>2357564.3468290311</v>
-      </c>
-      <c r="J32" s="1">
-        <f>B32/52</f>
-        <v>-698.54722586583864</v>
+        <v>-807.2537033823545</v>
       </c>
       <c r="K32" s="9">
-        <f>K31*(1+rental_growth)</f>
-        <v>1896.2119451909853</v>
+        <f t="shared" si="8"/>
+        <v>624.92609520000019</v>
       </c>
       <c r="L32" s="2">
         <v>0</v>
       </c>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
+      <c r="M32" s="2">
+        <f t="shared" si="9"/>
+        <v>6329.111519962692</v>
+      </c>
+      <c r="N32" s="8">
+        <f t="shared" si="10"/>
+        <v>-9481.0356254824255</v>
+      </c>
       <c r="O32" s="2"/>
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="B33" s="3">
         <f t="shared" si="0"/>
-        <v>-36324.45574502361</v>
+        <v>-41977.192575882436</v>
       </c>
       <c r="C33" s="3">
         <f t="shared" si="1"/>
-        <v>-25607.307953188963</v>
+        <v>-10904.007553743199</v>
       </c>
       <c r="D33" s="3">
         <f t="shared" si="2"/>
-        <v>-10717.14779183465</v>
+        <v>-31073.185022139231</v>
       </c>
       <c r="E33" s="3">
+        <f t="shared" si="11"/>
+        <v>549983.80873035837</v>
+      </c>
+      <c r="F33" s="3">
+        <f t="shared" si="4"/>
+        <v>34445.926367424014</v>
+      </c>
+      <c r="G33" s="8">
         <f t="shared" si="5"/>
-        <v>153011.82191072183</v>
-      </c>
-      <c r="F33" s="3">
+        <v>-1316.6292040305761</v>
+      </c>
+      <c r="H33" s="8">
+        <f t="shared" si="6"/>
+        <v>1063889.3341920001</v>
+      </c>
+      <c r="I33" s="8">
+        <f t="shared" si="7"/>
+        <v>513905.52546164172</v>
+      </c>
+      <c r="J33" s="1">
         <f t="shared" si="3"/>
-        <v>105505.23263042641</v>
-      </c>
-      <c r="G33" s="8">
-        <f>B33+F33</f>
-        <v>69180.776885402796</v>
-      </c>
-      <c r="H33" s="8">
-        <f>H32*(1+cap_appreciation_rate)</f>
-        <v>2713716.320061448</v>
-      </c>
-      <c r="I33" s="8">
-        <f t="shared" si="4"/>
-        <v>2560704.4981507263</v>
-      </c>
-      <c r="J33" s="1">
-        <f>B33/52</f>
-        <v>-698.54722586583864</v>
+        <v>-807.2537033823545</v>
       </c>
       <c r="K33" s="9">
-        <f>K32*(1+rental_growth)</f>
-        <v>2028.9467813543542</v>
+        <f t="shared" si="8"/>
+        <v>662.42166091200022</v>
       </c>
       <c r="L33" s="2">
         <v>0</v>
       </c>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
+      <c r="M33" s="2">
+        <f t="shared" si="9"/>
+        <v>6214.6370044278465</v>
+      </c>
+      <c r="N33" s="8">
+        <f t="shared" si="10"/>
+        <v>-7531.2662084584226</v>
+      </c>
       <c r="O33" s="2"/>
       <c r="P33" s="2"/>
       <c r="Q33" s="2"/>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="B34" s="3">
         <f t="shared" si="0"/>
-        <v>-36324.45574502361</v>
+        <v>-41977.192575882436</v>
       </c>
       <c r="C34" s="3">
         <f t="shared" si="1"/>
-        <v>-27143.746430380299</v>
+        <v>-11508.089572220571</v>
       </c>
       <c r="D34" s="3">
         <f t="shared" si="2"/>
-        <v>-9180.7093146433144</v>
+        <v>-30469.103003661865</v>
       </c>
       <c r="E34" s="3">
+        <f t="shared" si="11"/>
+        <v>538475.7191581378</v>
+      </c>
+      <c r="F34" s="3">
+        <f t="shared" si="4"/>
+        <v>36512.68194946945</v>
+      </c>
+      <c r="G34" s="8">
         <f t="shared" si="5"/>
-        <v>125868.07548034153</v>
-      </c>
-      <c r="F34" s="3">
+        <v>629.30997431938704</v>
+      </c>
+      <c r="H34" s="8">
+        <f t="shared" si="6"/>
+        <v>1127722.6942435203</v>
+      </c>
+      <c r="I34" s="8">
+        <f t="shared" si="7"/>
+        <v>589246.97508538247</v>
+      </c>
+      <c r="J34" s="1">
         <f t="shared" si="3"/>
-        <v>112890.59891455629</v>
-      </c>
-      <c r="G34" s="8">
-        <f>B34+F34</f>
-        <v>76566.143169532676</v>
-      </c>
-      <c r="H34" s="8">
-        <f>H33*(1+cap_appreciation_rate)</f>
-        <v>2903676.4624657496</v>
-      </c>
-      <c r="I34" s="8">
-        <f t="shared" si="4"/>
-        <v>2777808.3869854081</v>
-      </c>
-      <c r="J34" s="1">
-        <f>B34/52</f>
-        <v>-698.54722586583864</v>
+        <v>-807.2537033823545</v>
       </c>
       <c r="K34" s="9">
-        <f>K33*(1+rental_growth)</f>
-        <v>2170.9730560491594</v>
+        <f t="shared" si="8"/>
+        <v>702.16696056672026</v>
       </c>
       <c r="L34" s="2">
         <v>0</v>
       </c>
-      <c r="M34" s="2"/>
-      <c r="N34" s="2"/>
+      <c r="M34" s="2">
+        <f t="shared" si="9"/>
+        <v>6093.8206007323734</v>
+      </c>
+      <c r="N34" s="8">
+        <f t="shared" si="10"/>
+        <v>-5464.5106264129863</v>
+      </c>
       <c r="O34" s="2"/>
       <c r="P34" s="2"/>
       <c r="Q34" s="2"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="B35" s="3">
         <f t="shared" si="0"/>
-        <v>-36324.45574502361</v>
+        <v>-41977.192575882436</v>
       </c>
       <c r="C35" s="3">
         <f t="shared" si="1"/>
-        <v>-28772.371216203119</v>
+        <v>-12145.637734521591</v>
       </c>
       <c r="D35" s="3">
         <f t="shared" si="2"/>
-        <v>-7552.0845288204964</v>
+        <v>-29831.554841360845</v>
       </c>
       <c r="E35" s="3">
+        <f t="shared" si="11"/>
+        <v>526330.08142361615</v>
+      </c>
+      <c r="F35" s="3">
+        <f t="shared" si="4"/>
+        <v>38703.442866437625</v>
+      </c>
+      <c r="G35" s="8">
         <f t="shared" si="5"/>
-        <v>97095.704264138418</v>
-      </c>
-      <c r="F35" s="3">
+        <v>2692.561258827358</v>
+      </c>
+      <c r="H35" s="8">
+        <f t="shared" si="6"/>
+        <v>1195386.0558981316</v>
+      </c>
+      <c r="I35" s="8">
+        <f t="shared" si="7"/>
+        <v>669055.97447451542</v>
+      </c>
+      <c r="J35" s="1">
         <f t="shared" si="3"/>
-        <v>120792.94083857523</v>
-      </c>
-      <c r="G35" s="8">
-        <f>B35+F35</f>
-        <v>84468.48509355163</v>
-      </c>
-      <c r="H35" s="8">
-        <f>H34*(1+cap_appreciation_rate)</f>
-        <v>3106933.8148383521</v>
-      </c>
-      <c r="I35" s="8">
-        <f t="shared" si="4"/>
-        <v>3009838.1105742138</v>
-      </c>
-      <c r="J35" s="1">
-        <f>B35/52</f>
-        <v>-698.54722586583864</v>
+        <v>-807.2537033823545</v>
       </c>
       <c r="K35" s="9">
-        <f>K34*(1+rental_growth)</f>
-        <v>2322.9411699726006</v>
+        <f t="shared" si="8"/>
+        <v>744.29697820072352</v>
       </c>
       <c r="L35" s="2">
         <v>0</v>
       </c>
-      <c r="M35" s="2"/>
-      <c r="N35" s="2"/>
+      <c r="M35" s="2">
+        <f t="shared" si="9"/>
+        <v>5966.3109682721697</v>
+      </c>
+      <c r="N35" s="8">
+        <f t="shared" si="10"/>
+        <v>-3273.7497094448117</v>
+      </c>
       <c r="O35" s="2"/>
       <c r="P35" s="2"/>
       <c r="Q35" s="2"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="B36" s="3">
         <f t="shared" si="0"/>
-        <v>-36324.45574502361</v>
+        <v>-41977.192575882436</v>
       </c>
       <c r="C36" s="3">
         <f t="shared" si="1"/>
-        <v>-30498.713489175301</v>
+        <v>-12818.506065014088</v>
       </c>
       <c r="D36" s="3">
         <f t="shared" si="2"/>
-        <v>-5825.7422558483086</v>
+        <v>-29158.686510868345</v>
       </c>
       <c r="E36" s="3">
+        <f t="shared" si="11"/>
+        <v>513511.57535860204</v>
+      </c>
+      <c r="F36" s="3">
+        <f t="shared" si="4"/>
+        <v>41025.649438423883</v>
+      </c>
+      <c r="G36" s="8">
         <f t="shared" si="5"/>
-        <v>66596.990774963109</v>
-      </c>
-      <c r="F36" s="3">
+        <v>4880.1941647151161</v>
+      </c>
+      <c r="H36" s="8">
+        <f t="shared" si="6"/>
+        <v>1267109.2192520194</v>
+      </c>
+      <c r="I36" s="8">
+        <f t="shared" si="7"/>
+        <v>753597.64389341744</v>
+      </c>
+      <c r="J36" s="1">
         <f t="shared" si="3"/>
-        <v>129248.44669727552</v>
-      </c>
-      <c r="G36" s="8">
-        <f>B36+F36</f>
-        <v>92923.990952251916</v>
-      </c>
-      <c r="H36" s="8">
-        <f>H35*(1+cap_appreciation_rate)</f>
-        <v>3324419.181877037</v>
-      </c>
-      <c r="I36" s="8">
-        <f t="shared" si="4"/>
-        <v>3257822.191102074</v>
-      </c>
-      <c r="J36" s="1">
-        <f>B36/52</f>
-        <v>-698.54722586583864</v>
+        <v>-807.2537033823545</v>
       </c>
       <c r="K36" s="9">
-        <f>K35*(1+rental_growth)</f>
-        <v>2485.5470518706829</v>
+        <f t="shared" si="8"/>
+        <v>788.95479689276692</v>
       </c>
       <c r="L36" s="2">
         <v>0</v>
       </c>
-      <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
+      <c r="M36" s="2">
+        <f t="shared" si="9"/>
+        <v>5831.7373021736694</v>
+      </c>
+      <c r="N36" s="8">
+        <f t="shared" si="10"/>
+        <v>-951.54313745855325</v>
+      </c>
       <c r="O36" s="2"/>
       <c r="P36" s="2"/>
       <c r="Q36" s="2"/>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="B37" s="3">
         <f t="shared" si="0"/>
-        <v>-36324.45574502361</v>
+        <v>-41977.192575882436</v>
       </c>
       <c r="C37" s="3">
         <f t="shared" si="1"/>
-        <v>-32328.636298525824</v>
+        <v>-13528.651301015869</v>
       </c>
       <c r="D37" s="3">
         <f t="shared" si="2"/>
-        <v>-3995.819446497791</v>
+        <v>-28448.541274866566</v>
       </c>
       <c r="E37" s="3">
+        <f t="shared" si="11"/>
+        <v>499982.92405758618</v>
+      </c>
+      <c r="F37" s="3">
+        <f t="shared" si="4"/>
+        <v>43487.188404729313</v>
+      </c>
+      <c r="G37" s="8">
         <f t="shared" si="5"/>
-        <v>34268.354476437285</v>
-      </c>
-      <c r="F37" s="3">
+        <v>7199.7040838201901</v>
+      </c>
+      <c r="H37" s="8">
+        <f t="shared" si="6"/>
+        <v>1343135.7724071406</v>
+      </c>
+      <c r="I37" s="8">
+        <f t="shared" si="7"/>
+        <v>843152.84834955446</v>
+      </c>
+      <c r="J37" s="1">
         <f t="shared" si="3"/>
-        <v>138295.8379660848</v>
-      </c>
-      <c r="G37" s="8">
-        <f>B37+F37</f>
-        <v>101971.38222106118</v>
-      </c>
-      <c r="H37" s="8">
-        <f>H36*(1+cap_appreciation_rate)</f>
-        <v>3557128.52460843</v>
-      </c>
-      <c r="I37" s="8">
-        <f t="shared" si="4"/>
-        <v>3522860.1701319925</v>
-      </c>
-      <c r="J37" s="1">
-        <f>B37/52</f>
-        <v>-698.54722586583864</v>
+        <v>-807.2537033823545</v>
       </c>
       <c r="K37" s="9">
-        <f>K36*(1+rental_growth)</f>
-        <v>2659.5353455016307</v>
+        <f t="shared" si="8"/>
+        <v>836.29208470633296</v>
       </c>
       <c r="L37" s="2">
         <v>0</v>
       </c>
-      <c r="M37" s="2"/>
-      <c r="N37" s="2"/>
+      <c r="M37" s="2">
+        <f t="shared" si="9"/>
+        <v>5689.7082549733132</v>
+      </c>
+      <c r="N37" s="8">
+        <f t="shared" si="10"/>
+        <v>1509.995828846877</v>
+      </c>
       <c r="O37" s="2"/>
       <c r="P37" s="2"/>
       <c r="Q37" s="2"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B38" s="3">
         <f t="shared" si="0"/>
-        <v>-36324.45574502361</v>
+        <v>-41977.192575882436</v>
       </c>
       <c r="C38" s="3">
         <f t="shared" si="1"/>
-        <v>-34268.354476437373</v>
+        <v>-14278.138583092148</v>
       </c>
       <c r="D38" s="3">
         <f t="shared" si="2"/>
-        <v>-2056.101268586242</v>
+        <v>-27699.053992790283</v>
       </c>
       <c r="E38" s="3">
+        <f t="shared" si="11"/>
+        <v>485704.78547449404</v>
+      </c>
+      <c r="F38" s="3">
+        <f t="shared" si="4"/>
+        <v>46096.419709013076</v>
+      </c>
+      <c r="G38" s="8">
         <f t="shared" si="5"/>
-        <v>-8.7311491370201111E-11</v>
-      </c>
-      <c r="F38" s="3">
+        <v>9659.0379316886974</v>
+      </c>
+      <c r="H38" s="8">
+        <f t="shared" si="6"/>
+        <v>1423723.918751569</v>
+      </c>
+      <c r="I38" s="8">
+        <f t="shared" si="7"/>
+        <v>938019.1332770749</v>
+      </c>
+      <c r="J38" s="1">
         <f t="shared" si="3"/>
-        <v>147976.54662371075</v>
-      </c>
-      <c r="G38" s="8">
-        <f>B38+F38</f>
-        <v>111652.09087868713</v>
-      </c>
-      <c r="H38" s="8">
-        <f>H37*(1+cap_appreciation_rate)</f>
-        <v>3806127.5213310202</v>
-      </c>
-      <c r="I38" s="8">
-        <f t="shared" si="4"/>
-        <v>3806127.5213310202</v>
-      </c>
-      <c r="J38" s="1">
-        <f>B38/52</f>
-        <v>-698.54722586583864</v>
+        <v>-807.2537033823545</v>
       </c>
       <c r="K38" s="9">
-        <f>K37*(1+rental_growth)</f>
-        <v>2845.702819686745</v>
+        <f t="shared" si="8"/>
+        <v>886.469609788713</v>
       </c>
       <c r="L38" s="2">
         <v>0</v>
       </c>
-      <c r="M38" s="2"/>
-      <c r="N38" s="2"/>
+      <c r="M38" s="2">
+        <f t="shared" si="9"/>
+        <v>5539.8107985580573</v>
+      </c>
+      <c r="N38" s="8">
+        <f t="shared" si="10"/>
+        <v>4119.2271331306401</v>
+      </c>
       <c r="O38" s="2"/>
       <c r="P38" s="2"/>
       <c r="Q38" s="2"/>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="K39" s="1"/>
-      <c r="L39" s="2"/>
-      <c r="M39" s="2"/>
-      <c r="N39" s="2"/>
+      <c r="A39">
+        <v>12</v>
+      </c>
+      <c r="B39" s="3">
+        <f t="shared" si="0"/>
+        <v>-41977.192575882436</v>
+      </c>
+      <c r="C39" s="3">
+        <f t="shared" si="1"/>
+        <v>-15069.147460595455</v>
+      </c>
+      <c r="D39" s="3">
+        <f t="shared" si="2"/>
+        <v>-26908.045115286979</v>
+      </c>
+      <c r="E39" s="3">
+        <f t="shared" si="11"/>
+        <v>470635.63801389857</v>
+      </c>
+      <c r="F39" s="3">
+        <f t="shared" si="4"/>
+        <v>48862.204891553862</v>
+      </c>
+      <c r="G39" s="8">
+        <f t="shared" si="5"/>
+        <v>12266.621338728823</v>
+      </c>
+      <c r="H39" s="8">
+        <f t="shared" si="6"/>
+        <v>1509147.3538766631</v>
+      </c>
+      <c r="I39" s="8">
+        <f t="shared" si="7"/>
+        <v>1038511.7158627645</v>
+      </c>
+      <c r="J39" s="1">
+        <f t="shared" si="3"/>
+        <v>-807.2537033823545</v>
+      </c>
+      <c r="K39" s="9">
+        <f t="shared" si="8"/>
+        <v>939.6577863760358</v>
+      </c>
+      <c r="L39" s="2">
+        <v>0</v>
+      </c>
+      <c r="M39" s="2">
+        <f t="shared" si="9"/>
+        <v>5381.6090230573964</v>
+      </c>
+      <c r="N39" s="8">
+        <f t="shared" si="10"/>
+        <v>6885.0123156714253</v>
+      </c>
       <c r="O39" s="2"/>
       <c r="P39" s="2"/>
       <c r="Q39" s="2"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="K40" s="1"/>
-      <c r="L40" s="2"/>
-      <c r="M40" s="2"/>
-      <c r="N40" s="2"/>
+      <c r="A40">
+        <v>13</v>
+      </c>
+      <c r="B40" s="3">
+        <f t="shared" si="0"/>
+        <v>-41977.192575882436</v>
+      </c>
+      <c r="C40" s="3">
+        <f t="shared" si="1"/>
+        <v>-15903.978229912438</v>
+      </c>
+      <c r="D40" s="3">
+        <f t="shared" si="2"/>
+        <v>-26073.214345969995</v>
+      </c>
+      <c r="E40" s="3">
+        <f t="shared" si="11"/>
+        <v>454731.65978398611</v>
+      </c>
+      <c r="F40" s="3">
+        <f t="shared" si="4"/>
+        <v>51793.937185047092</v>
+      </c>
+      <c r="G40" s="8">
+        <f t="shared" si="5"/>
+        <v>15031.387478358654</v>
+      </c>
+      <c r="H40" s="8">
+        <f t="shared" si="6"/>
+        <v>1599696.1951092631</v>
+      </c>
+      <c r="I40" s="8">
+        <f t="shared" si="7"/>
+        <v>1144964.5353252769</v>
+      </c>
+      <c r="J40" s="1">
+        <f t="shared" si="3"/>
+        <v>-807.2537033823545</v>
+      </c>
+      <c r="K40" s="9">
+        <f t="shared" si="8"/>
+        <v>996.03725355859797</v>
+      </c>
+      <c r="L40" s="2">
+        <v>0</v>
+      </c>
+      <c r="M40" s="2">
+        <f t="shared" si="9"/>
+        <v>5214.6428691939991</v>
+      </c>
+      <c r="N40" s="8">
+        <f t="shared" si="10"/>
+        <v>9816.7446091646561</v>
+      </c>
       <c r="O40" s="2"/>
       <c r="P40" s="2"/>
       <c r="Q40" s="2"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="K41" s="1"/>
-      <c r="L41" s="2"/>
-      <c r="M41" s="2"/>
-      <c r="N41" s="2"/>
+      <c r="A41">
+        <v>14</v>
+      </c>
+      <c r="B41" s="3">
+        <f t="shared" si="0"/>
+        <v>-41977.192575882436</v>
+      </c>
+      <c r="C41" s="3">
+        <f t="shared" si="1"/>
+        <v>-16785.058623849593</v>
+      </c>
+      <c r="D41" s="3">
+        <f t="shared" si="2"/>
+        <v>-25192.133952032844</v>
+      </c>
+      <c r="E41" s="3">
+        <f t="shared" si="11"/>
+        <v>437946.60116013652</v>
+      </c>
+      <c r="F41" s="3">
+        <f t="shared" si="4"/>
+        <v>54901.57341614992</v>
+      </c>
+      <c r="G41" s="8">
+        <f t="shared" si="5"/>
+        <v>17962.807630674055</v>
+      </c>
+      <c r="H41" s="8">
+        <f t="shared" si="6"/>
+        <v>1695677.966815819</v>
+      </c>
+      <c r="I41" s="8">
+        <f t="shared" si="7"/>
+        <v>1257731.3656556825</v>
+      </c>
+      <c r="J41" s="1">
+        <f t="shared" si="3"/>
+        <v>-807.2537033823545</v>
+      </c>
+      <c r="K41" s="9">
+        <f t="shared" si="8"/>
+        <v>1055.7994887721138</v>
+      </c>
+      <c r="L41" s="2">
+        <v>0</v>
+      </c>
+      <c r="M41" s="2">
+        <f t="shared" si="9"/>
+        <v>5038.4267904065691</v>
+      </c>
+      <c r="N41" s="8">
+        <f t="shared" si="10"/>
+        <v>12924.380840267484</v>
+      </c>
       <c r="O41" s="2"/>
       <c r="P41" s="2"/>
       <c r="Q41" s="2"/>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="K42" s="1"/>
-      <c r="L42" s="2"/>
-      <c r="M42" s="2"/>
-      <c r="N42" s="2"/>
+      <c r="A42">
+        <v>15</v>
+      </c>
+      <c r="B42" s="3">
+        <f t="shared" si="0"/>
+        <v>-41977.192575882436</v>
+      </c>
+      <c r="C42" s="3">
+        <f t="shared" si="1"/>
+        <v>-17714.950871610858</v>
+      </c>
+      <c r="D42" s="3">
+        <f t="shared" si="2"/>
+        <v>-24262.241704271575</v>
+      </c>
+      <c r="E42" s="3">
+        <f t="shared" si="11"/>
+        <v>420231.65028852568</v>
+      </c>
+      <c r="F42" s="3">
+        <f t="shared" si="4"/>
+        <v>58195.667821118914</v>
+      </c>
+      <c r="G42" s="8">
+        <f t="shared" si="5"/>
+        <v>21070.923586090794</v>
+      </c>
+      <c r="H42" s="8">
+        <f t="shared" si="6"/>
+        <v>1797418.6448247682</v>
+      </c>
+      <c r="I42" s="8">
+        <f t="shared" si="7"/>
+        <v>1377186.9945362424</v>
+      </c>
+      <c r="J42" s="1">
+        <f t="shared" si="3"/>
+        <v>-807.2537033823545</v>
+      </c>
+      <c r="K42" s="9">
+        <f t="shared" si="8"/>
+        <v>1119.1474580984407</v>
+      </c>
+      <c r="L42" s="2">
+        <v>0</v>
+      </c>
+      <c r="M42" s="2">
+        <f t="shared" si="9"/>
+        <v>4852.4483408543156</v>
+      </c>
+      <c r="N42" s="8">
+        <f t="shared" si="10"/>
+        <v>16218.475245236477</v>
+      </c>
       <c r="O42" s="2"/>
       <c r="P42" s="2"/>
       <c r="Q42" s="2"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="K43" s="1"/>
+      <c r="A43">
+        <v>16</v>
+      </c>
+      <c r="B43" s="3">
+        <f t="shared" si="0"/>
+        <v>-41977.192575882436</v>
+      </c>
+      <c r="C43" s="3">
+        <f t="shared" si="1"/>
+        <v>-18696.3591498981</v>
+      </c>
+      <c r="D43" s="3">
+        <f t="shared" si="2"/>
+        <v>-23280.833425984336</v>
+      </c>
+      <c r="E43" s="3">
+        <f t="shared" si="11"/>
+        <v>401535.29113862757</v>
+      </c>
+      <c r="F43" s="3">
+        <f t="shared" si="4"/>
+        <v>61687.407890386057</v>
+      </c>
+      <c r="G43" s="8">
+        <f t="shared" si="5"/>
+        <v>24366.38199970049</v>
+      </c>
+      <c r="H43" s="8">
+        <f t="shared" si="6"/>
+        <v>1905263.7635142545</v>
+      </c>
+      <c r="I43" s="8">
+        <f t="shared" si="7"/>
+        <v>1503728.4723756269</v>
+      </c>
+      <c r="J43" s="1">
+        <f t="shared" si="3"/>
+        <v>-807.2537033823545</v>
+      </c>
+      <c r="K43" s="9">
+        <f t="shared" si="8"/>
+        <v>1186.2963055843472</v>
+      </c>
+      <c r="L43" s="2">
+        <v>0</v>
+      </c>
+      <c r="M43" s="2">
+        <f t="shared" si="9"/>
+        <v>4656.1666851968675</v>
+      </c>
+      <c r="N43" s="8">
+        <f t="shared" si="10"/>
+        <v>19710.215314503621</v>
+      </c>
+      <c r="O43" s="2"/>
+      <c r="P43" s="2"/>
       <c r="Q43" s="2"/>
     </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>17</v>
+      </c>
+      <c r="B44" s="3">
+        <f t="shared" si="0"/>
+        <v>-41977.192575882436</v>
+      </c>
+      <c r="C44" s="3">
+        <f t="shared" si="1"/>
+        <v>-19732.137446802455</v>
+      </c>
+      <c r="D44" s="3">
+        <f t="shared" si="2"/>
+        <v>-22245.055129079978</v>
+      </c>
+      <c r="E44" s="3">
+        <f t="shared" si="11"/>
+        <v>381803.15369182511</v>
+      </c>
+      <c r="F44" s="3">
+        <f t="shared" si="4"/>
+        <v>65388.652363809219</v>
+      </c>
+      <c r="G44" s="8">
+        <f t="shared" si="5"/>
+        <v>27860.470813742777</v>
+      </c>
+      <c r="H44" s="8">
+        <f t="shared" si="6"/>
+        <v>2019579.5893251097</v>
+      </c>
+      <c r="I44" s="8">
+        <f t="shared" si="7"/>
+        <v>1637776.4356332845</v>
+      </c>
+      <c r="J44" s="1">
+        <f t="shared" si="3"/>
+        <v>-807.2537033823545</v>
+      </c>
+      <c r="K44" s="9">
+        <f t="shared" si="8"/>
+        <v>1257.474083919408</v>
+      </c>
+      <c r="L44" s="2">
+        <v>0</v>
+      </c>
+      <c r="M44" s="2">
+        <f t="shared" si="9"/>
+        <v>4449.0110258159957</v>
+      </c>
+      <c r="N44" s="8">
+        <f t="shared" si="10"/>
+        <v>23411.459787926782</v>
+      </c>
+      <c r="O44" s="2"/>
+      <c r="P44" s="2"/>
+      <c r="Q44" s="2"/>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>18</v>
+      </c>
+      <c r="B45" s="3">
+        <f t="shared" si="0"/>
+        <v>-41977.192575882436</v>
+      </c>
+      <c r="C45" s="3">
+        <f t="shared" si="1"/>
+        <v>-20825.297861355306</v>
+      </c>
+      <c r="D45" s="3">
+        <f t="shared" si="2"/>
+        <v>-21151.894714527127</v>
+      </c>
+      <c r="E45" s="3">
+        <f t="shared" si="11"/>
+        <v>360977.85583046981</v>
+      </c>
+      <c r="F45" s="3">
+        <f t="shared" si="4"/>
+        <v>69311.971505637775</v>
+      </c>
+      <c r="G45" s="8">
+        <f t="shared" si="5"/>
+        <v>31565.157872660766</v>
+      </c>
+      <c r="H45" s="8">
+        <f t="shared" si="6"/>
+        <v>2140754.3646846162</v>
+      </c>
+      <c r="I45" s="8">
+        <f t="shared" si="7"/>
+        <v>1779776.5088541463</v>
+      </c>
+      <c r="J45" s="1">
+        <f t="shared" si="3"/>
+        <v>-807.2537033823545</v>
+      </c>
+      <c r="K45" s="9">
+        <f t="shared" si="8"/>
+        <v>1332.9225289545725</v>
+      </c>
+      <c r="L45" s="2">
+        <v>0</v>
+      </c>
+      <c r="M45" s="2">
+        <f t="shared" si="9"/>
+        <v>4230.3789429054259</v>
+      </c>
+      <c r="N45" s="8">
+        <f t="shared" si="10"/>
+        <v>27334.778929755339</v>
+      </c>
+      <c r="O45" s="2"/>
+      <c r="P45" s="2"/>
+      <c r="Q45" s="2"/>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>19</v>
+      </c>
+      <c r="B46" s="3">
+        <f t="shared" si="0"/>
+        <v>-41977.192575882436</v>
+      </c>
+      <c r="C46" s="3">
+        <f t="shared" si="1"/>
+        <v>-21979.019362874391</v>
+      </c>
+      <c r="D46" s="3">
+        <f t="shared" si="2"/>
+        <v>-19998.173213008042</v>
+      </c>
+      <c r="E46" s="3">
+        <f t="shared" si="11"/>
+        <v>338998.83646759542</v>
+      </c>
+      <c r="F46" s="3">
+        <f t="shared" si="4"/>
+        <v>73470.689795976039</v>
+      </c>
+      <c r="G46" s="8">
+        <f t="shared" si="5"/>
+        <v>35493.131862695212</v>
+      </c>
+      <c r="H46" s="8">
+        <f t="shared" si="6"/>
+        <v>2269199.6265656934</v>
+      </c>
+      <c r="I46" s="8">
+        <f t="shared" si="7"/>
+        <v>1930200.7900980981</v>
+      </c>
+      <c r="J46" s="1">
+        <f t="shared" si="3"/>
+        <v>-807.2537033823545</v>
+      </c>
+      <c r="K46" s="9">
+        <f t="shared" si="8"/>
+        <v>1412.8978806918469</v>
+      </c>
+      <c r="L46" s="2">
+        <v>0</v>
+      </c>
+      <c r="M46" s="2">
+        <f t="shared" si="9"/>
+        <v>3999.6346426016084</v>
+      </c>
+      <c r="N46" s="8">
+        <f t="shared" si="10"/>
+        <v>31493.497220093603</v>
+      </c>
+      <c r="O46" s="2"/>
+      <c r="P46" s="2"/>
+      <c r="Q46" s="2"/>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>20</v>
+      </c>
+      <c r="B47" s="3">
+        <f t="shared" si="0"/>
+        <v>-41977.192575882436</v>
+      </c>
+      <c r="C47" s="3">
+        <f t="shared" si="1"/>
+        <v>-23196.657035577631</v>
+      </c>
+      <c r="D47" s="3">
+        <f t="shared" si="2"/>
+        <v>-18780.535540304802</v>
+      </c>
+      <c r="E47" s="3">
+        <f t="shared" si="11"/>
+        <v>315802.17943201779</v>
+      </c>
+      <c r="F47" s="3">
+        <f t="shared" si="4"/>
+        <v>77878.931183734603</v>
+      </c>
+      <c r="G47" s="8">
+        <f t="shared" si="5"/>
+        <v>39657.845715913129</v>
+      </c>
+      <c r="H47" s="8">
+        <f t="shared" si="6"/>
+        <v>2405351.604159635</v>
+      </c>
+      <c r="I47" s="8">
+        <f t="shared" si="7"/>
+        <v>2089549.4247276173</v>
+      </c>
+      <c r="J47" s="1">
+        <f t="shared" si="3"/>
+        <v>-807.2537033823545</v>
+      </c>
+      <c r="K47" s="9">
+        <f t="shared" si="8"/>
+        <v>1497.6717535333578</v>
+      </c>
+      <c r="L47" s="2">
+        <v>0</v>
+      </c>
+      <c r="M47" s="2">
+        <f t="shared" si="9"/>
+        <v>3756.1071080609604</v>
+      </c>
+      <c r="N47" s="8">
+        <f t="shared" si="10"/>
+        <v>35901.738607852167</v>
+      </c>
+      <c r="O47" s="2"/>
+      <c r="P47" s="2"/>
+      <c r="Q47" s="2"/>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>21</v>
+      </c>
+      <c r="B48" s="3">
+        <f t="shared" si="0"/>
+        <v>-41977.192575882436</v>
+      </c>
+      <c r="C48" s="3">
+        <f t="shared" si="1"/>
+        <v>-24481.751835348634</v>
+      </c>
+      <c r="D48" s="3">
+        <f t="shared" si="2"/>
+        <v>-17495.440740533802</v>
+      </c>
+      <c r="E48" s="3">
+        <f t="shared" si="11"/>
+        <v>291320.42759666918</v>
+      </c>
+      <c r="F48" s="3">
+        <f t="shared" si="4"/>
+        <v>82551.667054758684</v>
+      </c>
+      <c r="G48" s="8">
+        <f t="shared" si="5"/>
+        <v>44073.56262698301</v>
+      </c>
+      <c r="H48" s="8">
+        <f t="shared" si="6"/>
+        <v>2549672.7004092131</v>
+      </c>
+      <c r="I48" s="8">
+        <f t="shared" si="7"/>
+        <v>2258352.2728125439</v>
+      </c>
+      <c r="J48" s="1">
+        <f t="shared" si="3"/>
+        <v>-807.2537033823545</v>
+      </c>
+      <c r="K48" s="9">
+        <f t="shared" si="8"/>
+        <v>1587.5320587453593</v>
+      </c>
+      <c r="L48" s="2">
+        <v>0</v>
+      </c>
+      <c r="M48" s="2">
+        <f t="shared" si="9"/>
+        <v>3499.0881481067609</v>
+      </c>
+      <c r="N48" s="8">
+        <f t="shared" si="10"/>
+        <v>40574.474478876247</v>
+      </c>
+      <c r="O48" s="2"/>
+      <c r="P48" s="2"/>
+      <c r="Q48" s="2"/>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>22</v>
+      </c>
+      <c r="B49" s="3">
+        <f t="shared" si="0"/>
+        <v>-41977.192575882436</v>
+      </c>
+      <c r="C49" s="3">
+        <f t="shared" si="1"/>
+        <v>-25838.040887026946</v>
+      </c>
+      <c r="D49" s="3">
+        <f t="shared" si="2"/>
+        <v>-16139.151688855485</v>
+      </c>
+      <c r="E49" s="3">
+        <f t="shared" si="11"/>
+        <v>265482.38670964225</v>
+      </c>
+      <c r="F49" s="3">
+        <f t="shared" si="4"/>
+        <v>87504.767078044213</v>
+      </c>
+      <c r="G49" s="8">
+        <f t="shared" si="5"/>
+        <v>48755.404839932875</v>
+      </c>
+      <c r="H49" s="8">
+        <f t="shared" si="6"/>
+        <v>2702653.0624337662</v>
+      </c>
+      <c r="I49" s="8">
+        <f t="shared" si="7"/>
+        <v>2437170.6757241241</v>
+      </c>
+      <c r="J49" s="1">
+        <f t="shared" si="3"/>
+        <v>-807.2537033823545</v>
+      </c>
+      <c r="K49" s="9">
+        <f t="shared" si="8"/>
+        <v>1682.783982270081</v>
+      </c>
+      <c r="L49" s="2">
+        <v>0</v>
+      </c>
+      <c r="M49" s="2">
+        <f t="shared" si="9"/>
+        <v>3227.8303377710972</v>
+      </c>
+      <c r="N49" s="8">
+        <f t="shared" si="10"/>
+        <v>45527.574502161777</v>
+      </c>
+      <c r="O49" s="2"/>
+      <c r="P49" s="2"/>
+      <c r="Q49" s="2"/>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>23</v>
+      </c>
+      <c r="B50" s="3">
+        <f t="shared" si="0"/>
+        <v>-41977.192575882436</v>
+      </c>
+      <c r="C50" s="3">
+        <f t="shared" si="1"/>
+        <v>-27269.468352168242</v>
+      </c>
+      <c r="D50" s="3">
+        <f t="shared" si="2"/>
+        <v>-14707.724223714193</v>
+      </c>
+      <c r="E50" s="3">
+        <f t="shared" si="11"/>
+        <v>238212.918357474</v>
+      </c>
+      <c r="F50" s="3">
+        <f t="shared" si="4"/>
+        <v>92755.053102726873</v>
+      </c>
+      <c r="G50" s="8">
+        <f t="shared" si="5"/>
+        <v>53719.405371587272</v>
+      </c>
+      <c r="H50" s="8">
+        <f t="shared" si="6"/>
+        <v>2864812.2461797921</v>
+      </c>
+      <c r="I50" s="8">
+        <f t="shared" si="7"/>
+        <v>2626599.3278223183</v>
+      </c>
+      <c r="J50" s="1">
+        <f t="shared" si="3"/>
+        <v>-807.2537033823545</v>
+      </c>
+      <c r="K50" s="9">
+        <f t="shared" si="8"/>
+        <v>1783.7510212062859</v>
+      </c>
+      <c r="L50" s="2">
+        <v>0</v>
+      </c>
+      <c r="M50" s="2">
+        <f t="shared" si="9"/>
+        <v>2941.5448447428389</v>
+      </c>
+      <c r="N50" s="8">
+        <f t="shared" si="10"/>
+        <v>50777.860526844437</v>
+      </c>
+      <c r="O50" s="2"/>
+      <c r="P50" s="2"/>
+      <c r="Q50" s="2"/>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>24</v>
+      </c>
+      <c r="B51" s="3">
+        <f t="shared" si="0"/>
+        <v>-41977.192575882436</v>
+      </c>
+      <c r="C51" s="3">
+        <f t="shared" si="1"/>
+        <v>-28780.196898878359</v>
+      </c>
+      <c r="D51" s="3">
+        <f t="shared" si="2"/>
+        <v>-13196.99567700407</v>
+      </c>
+      <c r="E51" s="3">
+        <f t="shared" si="11"/>
+        <v>209432.72145859565</v>
+      </c>
+      <c r="F51" s="3">
+        <f t="shared" si="4"/>
+        <v>98320.356288890485</v>
+      </c>
+      <c r="G51" s="8">
+        <f t="shared" si="5"/>
+        <v>58982.562848408867</v>
+      </c>
+      <c r="H51" s="8">
+        <f t="shared" si="6"/>
+        <v>3036700.98095058</v>
+      </c>
+      <c r="I51" s="8">
+        <f t="shared" si="7"/>
+        <v>2827268.2594919843</v>
+      </c>
+      <c r="J51" s="1">
+        <f t="shared" si="3"/>
+        <v>-807.2537033823545</v>
+      </c>
+      <c r="K51" s="9">
+        <f t="shared" si="8"/>
+        <v>1890.7760824786633</v>
+      </c>
+      <c r="L51" s="2">
+        <v>0</v>
+      </c>
+      <c r="M51" s="2">
+        <f t="shared" si="9"/>
+        <v>2639.399135400814</v>
+      </c>
+      <c r="N51" s="8">
+        <f t="shared" si="10"/>
+        <v>56343.163713008049</v>
+      </c>
+      <c r="O51" s="2"/>
+      <c r="P51" s="2"/>
+      <c r="Q51" s="2"/>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>25</v>
+      </c>
+      <c r="B52" s="3">
+        <f t="shared" si="0"/>
+        <v>-41977.192575882436</v>
+      </c>
+      <c r="C52" s="3">
+        <f t="shared" si="1"/>
+        <v>-30374.619807076226</v>
+      </c>
+      <c r="D52" s="3">
+        <f t="shared" si="2"/>
+        <v>-11602.572768806212</v>
+      </c>
+      <c r="E52" s="3">
+        <f t="shared" si="11"/>
+        <v>179058.10165151942</v>
+      </c>
+      <c r="F52" s="3">
+        <f t="shared" si="4"/>
+        <v>104219.57766622392</v>
+      </c>
+      <c r="G52" s="8">
+        <f t="shared" si="5"/>
+        <v>64562.899644102727</v>
+      </c>
+      <c r="H52" s="8">
+        <f t="shared" si="6"/>
+        <v>3218903.0398076149</v>
+      </c>
+      <c r="I52" s="8">
+        <f t="shared" si="7"/>
+        <v>3039844.9381560953</v>
+      </c>
+      <c r="J52" s="1">
+        <f t="shared" si="3"/>
+        <v>-807.2537033823545</v>
+      </c>
+      <c r="K52" s="9">
+        <f t="shared" si="8"/>
+        <v>2004.2226474273832</v>
+      </c>
+      <c r="L52" s="2">
+        <v>0</v>
+      </c>
+      <c r="M52" s="2">
+        <f t="shared" si="9"/>
+        <v>2320.5145537612425</v>
+      </c>
+      <c r="N52" s="8">
+        <f t="shared" si="10"/>
+        <v>62242.385090341486</v>
+      </c>
+      <c r="O52" s="2"/>
+      <c r="P52" s="2"/>
+      <c r="Q52" s="2"/>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>26</v>
+      </c>
+      <c r="B53" s="3">
+        <f t="shared" si="0"/>
+        <v>-41977.192575882436</v>
+      </c>
+      <c r="C53" s="3">
+        <f t="shared" si="1"/>
+        <v>-32057.373744388246</v>
+      </c>
+      <c r="D53" s="3">
+        <f t="shared" si="2"/>
+        <v>-9919.8188314941872</v>
+      </c>
+      <c r="E53" s="3">
+        <f t="shared" si="11"/>
+        <v>147000.72790713116</v>
+      </c>
+      <c r="F53" s="3">
+        <f t="shared" si="4"/>
+        <v>110472.75232619735</v>
+      </c>
+      <c r="G53" s="8">
+        <f t="shared" si="5"/>
+        <v>70479.523516613757</v>
+      </c>
+      <c r="H53" s="8">
+        <f t="shared" si="6"/>
+        <v>3412037.2221960719</v>
+      </c>
+      <c r="I53" s="8">
+        <f t="shared" si="7"/>
+        <v>3265036.4942889409</v>
+      </c>
+      <c r="J53" s="1">
+        <f t="shared" si="3"/>
+        <v>-807.2537033823545</v>
+      </c>
+      <c r="K53" s="9">
+        <f t="shared" si="8"/>
+        <v>2124.4760062730261</v>
+      </c>
+      <c r="L53" s="2">
+        <v>0</v>
+      </c>
+      <c r="M53" s="2">
+        <f t="shared" si="9"/>
+        <v>1983.9637662988375</v>
+      </c>
+      <c r="N53" s="8">
+        <f t="shared" si="10"/>
+        <v>68495.559750314918</v>
+      </c>
+      <c r="O53" s="2"/>
+      <c r="P53" s="2"/>
+      <c r="Q53" s="2"/>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>27</v>
+      </c>
+      <c r="B54" s="3">
+        <f t="shared" si="0"/>
+        <v>-41977.192575882436</v>
+      </c>
+      <c r="C54" s="3">
+        <f t="shared" si="1"/>
+        <v>-33833.352249827352</v>
+      </c>
+      <c r="D54" s="3">
+        <f t="shared" si="2"/>
+        <v>-8143.8403260550795</v>
+      </c>
+      <c r="E54" s="3">
+        <f t="shared" si="11"/>
+        <v>113167.37565730381</v>
+      </c>
+      <c r="F54" s="3">
+        <f t="shared" si="4"/>
+        <v>117101.11746576922</v>
+      </c>
+      <c r="G54" s="8">
+        <f t="shared" si="5"/>
+        <v>76752.692955097795</v>
+      </c>
+      <c r="H54" s="8">
+        <f t="shared" si="6"/>
+        <v>3616759.4555278365</v>
+      </c>
+      <c r="I54" s="8">
+        <f t="shared" si="7"/>
+        <v>3503592.0798705327</v>
+      </c>
+      <c r="J54" s="1">
+        <f t="shared" si="3"/>
+        <v>-807.2537033823545</v>
+      </c>
+      <c r="K54" s="9">
+        <f t="shared" si="8"/>
+        <v>2251.944566649408</v>
+      </c>
+      <c r="L54" s="2">
+        <v>0</v>
+      </c>
+      <c r="M54" s="2">
+        <f t="shared" si="9"/>
+        <v>1628.7680652110159</v>
+      </c>
+      <c r="N54" s="8">
+        <f t="shared" si="10"/>
+        <v>75123.924889886781</v>
+      </c>
+      <c r="O54" s="2"/>
+      <c r="P54" s="2"/>
+      <c r="Q54" s="2"/>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>28</v>
+      </c>
+      <c r="B55" s="3">
+        <f t="shared" si="0"/>
+        <v>-41977.192575882436</v>
+      </c>
+      <c r="C55" s="3">
+        <f t="shared" si="1"/>
+        <v>-35707.719964467789</v>
+      </c>
+      <c r="D55" s="3">
+        <f t="shared" si="2"/>
+        <v>-6269.4726114146451</v>
+      </c>
+      <c r="E55" s="3">
+        <f t="shared" si="11"/>
+        <v>77459.655692836022</v>
+      </c>
+      <c r="F55" s="3">
+        <f t="shared" si="4"/>
+        <v>124127.18451371536</v>
+      </c>
+      <c r="G55" s="8">
+        <f t="shared" si="5"/>
+        <v>83403.886460115857</v>
+      </c>
+      <c r="H55" s="8">
+        <f t="shared" si="6"/>
+        <v>3833765.0228595068</v>
+      </c>
+      <c r="I55" s="8">
+        <f t="shared" si="7"/>
+        <v>3756305.367166671</v>
+      </c>
+      <c r="J55" s="1">
+        <f t="shared" si="3"/>
+        <v>-807.2537033823545</v>
+      </c>
+      <c r="K55" s="9">
+        <f t="shared" si="8"/>
+        <v>2387.0612406483724</v>
+      </c>
+      <c r="L55" s="2">
+        <v>0</v>
+      </c>
+      <c r="M55" s="2">
+        <f t="shared" si="9"/>
+        <v>1253.8945222829291</v>
+      </c>
+      <c r="N55" s="8">
+        <f t="shared" si="10"/>
+        <v>82149.991937832921</v>
+      </c>
+      <c r="O55" s="2"/>
+      <c r="P55" s="2"/>
+      <c r="Q55" s="2"/>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>29</v>
+      </c>
+      <c r="B56" s="3">
+        <f t="shared" si="0"/>
+        <v>-41977.192575882436</v>
+      </c>
+      <c r="C56" s="3">
+        <f t="shared" si="1"/>
+        <v>-37685.927650499303</v>
+      </c>
+      <c r="D56" s="3">
+        <f t="shared" si="2"/>
+        <v>-4291.2649253831296</v>
+      </c>
+      <c r="E56" s="3">
+        <f t="shared" si="11"/>
+        <v>39773.728042336719</v>
+      </c>
+      <c r="F56" s="3">
+        <f t="shared" si="4"/>
+        <v>131574.8155845383</v>
+      </c>
+      <c r="G56" s="8">
+        <f t="shared" si="5"/>
+        <v>90455.875993732494</v>
+      </c>
+      <c r="H56" s="8">
+        <f t="shared" si="6"/>
+        <v>4063790.9242310775</v>
+      </c>
+      <c r="I56" s="8">
+        <f t="shared" si="7"/>
+        <v>4024017.1961887409</v>
+      </c>
+      <c r="J56" s="1">
+        <f t="shared" si="3"/>
+        <v>-807.2537033823545</v>
+      </c>
+      <c r="K56" s="9">
+        <f t="shared" si="8"/>
+        <v>2530.2849150872748</v>
+      </c>
+      <c r="L56" s="2">
+        <v>0</v>
+      </c>
+      <c r="M56" s="2">
+        <f t="shared" si="9"/>
+        <v>858.25298507662592</v>
+      </c>
+      <c r="N56" s="8">
+        <f t="shared" si="10"/>
+        <v>89597.623008655864</v>
+      </c>
+      <c r="O56" s="2"/>
+      <c r="P56" s="2"/>
+      <c r="Q56" s="2"/>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>30</v>
+      </c>
+      <c r="B57" s="3">
+        <f t="shared" si="0"/>
+        <v>-41977.192575882436</v>
+      </c>
+      <c r="C57" s="3">
+        <f t="shared" si="1"/>
+        <v>-39773.728042336967</v>
+      </c>
+      <c r="D57" s="3">
+        <f t="shared" si="2"/>
+        <v>-2203.4645335454679</v>
+      </c>
+      <c r="E57" s="3">
+        <f t="shared" si="11"/>
+        <v>-2.4738255888223648E-10</v>
+      </c>
+      <c r="F57" s="3">
+        <f t="shared" si="4"/>
+        <v>139469.3045196106</v>
+      </c>
+      <c r="G57" s="8">
+        <f t="shared" si="5"/>
+        <v>97932.804850437256</v>
+      </c>
+      <c r="H57" s="8">
+        <f t="shared" si="6"/>
+        <v>4307618.3796849428</v>
+      </c>
+      <c r="I57" s="8">
+        <f t="shared" si="7"/>
+        <v>4307618.3796849428</v>
+      </c>
+      <c r="J57" s="1">
+        <f t="shared" si="3"/>
+        <v>-807.2537033823545</v>
+      </c>
+      <c r="K57" s="9">
+        <f t="shared" si="8"/>
+        <v>2682.1020099925113</v>
+      </c>
+      <c r="L57" s="2">
+        <v>0</v>
+      </c>
+      <c r="M57" s="2">
+        <f t="shared" si="9"/>
+        <v>440.69290670909362</v>
+      </c>
+      <c r="N57" s="8">
+        <f t="shared" si="10"/>
+        <v>97492.11194372816</v>
+      </c>
+      <c r="O57" s="2"/>
+      <c r="P57" s="2"/>
+      <c r="Q57" s="2"/>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="K58" s="1"/>
+      <c r="L58" s="2"/>
+      <c r="M58" s="2"/>
+      <c r="O58" s="2"/>
+      <c r="P58" s="2"/>
+      <c r="Q58" s="2"/>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="K59" s="1"/>
+      <c r="L59" s="2"/>
+      <c r="M59" s="2"/>
+      <c r="O59" s="2"/>
+      <c r="P59" s="2"/>
+      <c r="Q59" s="2"/>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="K60" s="1"/>
+      <c r="L60" s="2"/>
+      <c r="M60" s="2"/>
+      <c r="O60" s="2"/>
+      <c r="P60" s="2"/>
+      <c r="Q60" s="2"/>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="K61" s="1"/>
+      <c r="L61" s="2"/>
+      <c r="M61" s="2"/>
+      <c r="O61" s="2"/>
+      <c r="P61" s="2"/>
+      <c r="Q61" s="2"/>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="K62" s="1"/>
+      <c r="Q62" s="2"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="G1:I1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+  <conditionalFormatting sqref="G1:I1048576 N1:N1048576">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
updated tax deduction cal
</commit_message>
<xml_diff>
--- a/single-calculation.xlsx
+++ b/single-calculation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\4047657\Documents\calculations\hmark\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bmj/Library/CloudStorage/GoogleDrive-bibinmjose@gmail.com/My Drive/🏡 Documents/InvestmentProperty/TBD/housemarket/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9C48A24-8298-4884-8624-1B56E13DC582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC8D5C09-B3D7-E047-98C0-F273EC515BCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{61E349DD-C396-4897-954F-94B6F0CC0F58}"/>
+    <workbookView xWindow="0" yWindow="800" windowWidth="36000" windowHeight="21320" xr2:uid="{61E349DD-C396-4897-954F-94B6F0CC0F58}"/>
   </bookViews>
   <sheets>
     <sheet name="finance" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -130,11 +129,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="0.000%"/>
-    <numFmt numFmtId="166" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="0.000%"/>
+    <numFmt numFmtId="168" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -179,32 +178,32 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Currency" xfId="3" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="2" builtinId="5"/>
+    <cellStyle name="Per cent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -231,7 +230,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -387,79 +386,79 @@
                 <c:formatCode>_-"$"* #,##0_-;\-"$"* #,##0_-;_-"$"* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>-14521.192575882436</c:v>
+                  <c:v>-12805.192575882436</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-12873.832575882432</c:v>
+                  <c:v>-11054.872575882433</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-11127.630975882428</c:v>
+                  <c:v>-9199.5333758824272</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-9276.6572798824309</c:v>
+                  <c:v>-7232.8738238824299</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-7314.6251621224292</c:v>
+                  <c:v>-5148.2146987624292</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-5234.8711172968251</c:v>
+                  <c:v>-2938.4760261352276</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-3030.3318297816877</c:v>
+                  <c:v>-596.15303315039637</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-693.52018501563725</c:v>
+                  <c:v>1886.70933941353</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1783.5001584363708</c:v>
+                  <c:v>4518.5434543312876</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4409.1417224955003</c:v>
+                  <c:v>7308.2876161441091</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7192.3217803981825</c:v>
+                  <c:v>10265.41642766571</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>10142.492641775025</c:v>
+                  <c:v>13399.972967878603</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13269.673754834475</c:v>
+                  <c:v>16722.602900504266</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>16584.485734677488</c:v>
+                  <c:v>20244.59062908747</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>20098.186433311093</c:v>
+                  <c:v>23977.897621385666</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>23822.709173862706</c:v>
+                  <c:v>27935.203033221755</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>27770.703278847417</c:v>
+                  <c:v>32129.946769768023</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>31955.577030131215</c:v>
+                  <c:v>36576.375130507047</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>36391.543206492031</c:v>
+                  <c:v>41289.589192890431</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>41093.667353434503</c:v>
+                  <c:v>46285.596099016795</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>46077.918949193525</c:v>
+                  <c:v>51581.363419510759</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>51361.225640698089</c:v>
+                  <c:v>57194.876779234342</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>56961.530733692925</c:v>
+                  <c:v>63145.200940541356</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>62897.854132267457</c:v>
+                  <c:v>69452.544551526778</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>69190.356934756448</c:v>
+                  <c:v>76138.328779171337</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -599,79 +598,79 @@
                 <c:formatCode>_-"$"* #,##0_-;\-"$"* #,##0_-;_-"$"* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>-7791.2005758824362</c:v>
+                  <c:v>-10244.154060705949</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-6236.1063128232099</c:v>
+                  <c:v>-8843.8980607059457</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-4587.2819715905016</c:v>
+                  <c:v>-7359.6267007059414</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-2839.0802344935082</c:v>
+                  <c:v>-5786.2990591059443</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-985.51364215973717</c:v>
+                  <c:v>-4118.571759009943</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>979.76588713102137</c:v>
+                  <c:v>-2350.7808209081822</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3063.4887709506856</c:v>
+                  <c:v>-476.92242652031712</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5272.7907832565324</c:v>
+                  <c:v>1509.3674715308239</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7615.2374606100402</c:v>
+                  <c:v>3614.8347634650299</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10098.849977468813</c:v>
+                  <c:v>5846.6300929152876</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>12732.13257895624</c:v>
+                  <c:v>8212.3331421325674</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>15524.101664832422</c:v>
+                  <c:v>10719.978374302882</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>18484.316624028474</c:v>
+                  <c:v>13378.082320403413</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>21622.912525084059</c:v>
+                  <c:v>16195.672503269976</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>24950.63477416541</c:v>
+                  <c:v>19182.318097108531</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>28478.875859059575</c:v>
+                  <c:v>22348.162426577404</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>32219.714304663412</c:v>
+                  <c:v>25703.957415814417</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>36185.955973036638</c:v>
+                  <c:v>29261.100104405639</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>40391.177849093641</c:v>
+                  <c:v>33031.671354312348</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44849.774461495464</c:v>
+                  <c:v>37028.476879213435</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>49577.007097300288</c:v>
+                  <c:v>41265.09073560861</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>54589.055978469187</c:v>
+                  <c:v>45755.901423387477</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>59903.075578435761</c:v>
+                  <c:v>50516.160752433083</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>65537.253267668275</c:v>
+                  <c:v>55562.035641221424</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>71510.871488517689</c:v>
+                  <c:v>60910.663023337067</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -744,79 +743,79 @@
                       <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
                       <c:ptCount val="25"/>
                       <c:pt idx="0">
-                        <c:v>6729.9920000000002</c:v>
+                        <c:v>2561.0385151764876</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>6637.7262630592222</c:v>
+                        <c:v>2210.9745151764869</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>6540.3490042919266</c:v>
+                        <c:v>1839.9066751764856</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>6437.5770453889227</c:v>
+                        <c:v>1446.5747647764861</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>6329.111519962692</c:v>
+                        <c:v>1029.642939752486</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>6214.6370044278465</c:v>
+                        <c:v>587.69520522704556</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>6093.8206007323734</c:v>
+                        <c:v>119.23060663007928</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>5966.3109682721697</c:v>
+                        <c:v>-377.34186788270603</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>5831.7373021736694</c:v>
+                        <c:v>-903.7086908662576</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>5689.7082549733132</c:v>
+                        <c:v>-1461.6575232288219</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>5539.8107985580573</c:v>
+                        <c:v>-2053.0832855331423</c:v>
                       </c:pt>
                       <c:pt idx="11">
-                        <c:v>5381.6090230573964</c:v>
+                        <c:v>-2679.9945935757205</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>5214.6428691939991</c:v>
+                        <c:v>-3344.5205801008533</c:v>
                       </c:pt>
                       <c:pt idx="13">
-                        <c:v>5038.4267904065691</c:v>
+                        <c:v>-4048.918125817494</c:v>
                       </c:pt>
                       <c:pt idx="14">
-                        <c:v>4852.4483408543156</c:v>
+                        <c:v>-4795.5795242771337</c:v>
                       </c:pt>
                       <c:pt idx="15">
-                        <c:v>4656.1666851968675</c:v>
+                        <c:v>-5587.0406066443511</c:v>
                       </c:pt>
                       <c:pt idx="16">
-                        <c:v>4449.0110258159957</c:v>
+                        <c:v>-6425.9893539536051</c:v>
                       </c:pt>
                       <c:pt idx="17">
-                        <c:v>4230.3789429054259</c:v>
+                        <c:v>-7315.2750261014098</c:v>
                       </c:pt>
                       <c:pt idx="18">
-                        <c:v>3999.6346426016084</c:v>
+                        <c:v>-8257.917838578087</c:v>
                       </c:pt>
                       <c:pt idx="19">
-                        <c:v>3756.1071080609604</c:v>
+                        <c:v>-9257.1192198033586</c:v>
                       </c:pt>
                       <c:pt idx="20">
-                        <c:v>3499.0881481067609</c:v>
+                        <c:v>-10316.272683902152</c:v>
                       </c:pt>
                       <c:pt idx="21">
-                        <c:v>3227.8303377710972</c:v>
+                        <c:v>-11438.975355846869</c:v>
                       </c:pt>
                       <c:pt idx="22">
-                        <c:v>2941.5448447428389</c:v>
+                        <c:v>-12629.040188108273</c:v>
                       </c:pt>
                       <c:pt idx="23">
-                        <c:v>2639.399135400814</c:v>
+                        <c:v>-13890.508910305356</c:v>
                       </c:pt>
                       <c:pt idx="24">
-                        <c:v>2320.5145537612425</c:v>
+                        <c:v>-15227.665755834269</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -977,79 +976,79 @@
                 <c:formatCode>_-"$"* #,##0_-;\-"$"* #,##0_-;_-"$"* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>795000</c:v>
+                  <c:v>784400</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>842700</c:v>
+                  <c:v>831464</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>893262</c:v>
+                  <c:v>881351.84000000008</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>946857.72000000009</c:v>
+                  <c:v>934232.95040000009</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1003669.1832000001</c:v>
+                  <c:v>990286.92742400011</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1063889.3341920001</c:v>
+                  <c:v>1049704.1430694403</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1127722.6942435203</c:v>
+                  <c:v>1112686.3916536067</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1195386.0558981316</c:v>
+                  <c:v>1179447.5751528232</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1267109.2192520194</c:v>
+                  <c:v>1250214.4296619927</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1343135.7724071406</c:v>
+                  <c:v>1325227.2954417123</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1423723.918751569</c:v>
+                  <c:v>1404740.933168215</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1509147.3538766631</c:v>
+                  <c:v>1489025.389158308</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1599696.1951092631</c:v>
+                  <c:v>1578366.9125078067</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1695677.966815819</c:v>
+                  <c:v>1673068.9272582752</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1797418.6448247682</c:v>
+                  <c:v>1773453.0628937718</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1905263.7635142545</c:v>
+                  <c:v>1879860.2466673981</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2019579.5893251097</c:v>
+                  <c:v>1992651.8614674422</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2140754.3646846162</c:v>
+                  <c:v>2112210.9731554887</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2269199.6265656934</c:v>
+                  <c:v>2238943.6315448182</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2405351.604159635</c:v>
+                  <c:v>2373280.2494375072</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2549672.7004092131</c:v>
+                  <c:v>2515677.0644037579</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2702653.0624337662</c:v>
+                  <c:v>2666617.6882679835</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2864812.2461797921</c:v>
+                  <c:v>2826614.7495640628</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3036700.98095058</c:v>
+                  <c:v>2996211.6345379069</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3218903.0398076149</c:v>
+                  <c:v>3175984.3326101815</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1204,79 +1203,79 @@
                 <c:formatCode>_-"$"* #,##0_-;\-"$"* #,##0_-;_-"$"* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>195927.23257588246</c:v>
+                  <c:v>185327.23257588246</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>252415.79383646883</c:v>
+                  <c:v>241179.79383646883</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>312253.24139089161</c:v>
+                  <c:v>300343.08139089169</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>375638.26873982954</c:v>
+                  <c:v>363013.49913982954</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>442781.36691589851</c:v>
+                  <c:v>429399.11113989854</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>513905.52546164172</c:v>
+                  <c:v>499720.33433908189</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>589246.97508538247</c:v>
+                  <c:v>574210.67249546887</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>669055.97447451542</c:v>
+                  <c:v>653117.49372920708</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>753597.64389341744</c:v>
+                  <c:v>736702.85430339072</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>843152.84834955446</c:v>
+                  <c:v>825244.37138412613</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>938019.1332770749</c:v>
+                  <c:v>919036.14769372088</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1038511.7158627645</c:v>
+                  <c:v>1018389.7511444094</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1144964.5353252769</c:v>
+                  <c:v>1123635.2527238205</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1257731.3656556825</c:v>
+                  <c:v>1235122.3260981387</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1377186.9945362424</c:v>
+                  <c:v>1353221.4126052461</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1503728.4723756269</c:v>
+                  <c:v>1478324.9555287706</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1637776.4356332845</c:v>
+                  <c:v>1610848.707775617</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1779776.5088541463</c:v>
+                  <c:v>1751233.1173250189</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1930200.7900980981</c:v>
+                  <c:v>1899944.7950772229</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2089549.4247276173</c:v>
+                  <c:v>2057478.0700054895</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2258352.2728125439</c:v>
+                  <c:v>2224356.6368070887</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2437170.6757241241</c:v>
+                  <c:v>2401135.3015583414</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2626599.3278223183</c:v>
+                  <c:v>2588401.831206589</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2827268.2594919843</c:v>
+                  <c:v>2786778.9130793111</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3039844.9381560953</c:v>
+                  <c:v>2996926.230958662</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2093,79 +2092,79 @@
                       <c:formatCode>#,##0</c:formatCode>
                       <c:ptCount val="25"/>
                       <c:pt idx="0">
-                        <c:v>27456</c:v>
+                        <c:v>29172</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>29103.360000000004</c:v>
+                        <c:v>30922.320000000003</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>30849.561600000008</c:v>
+                        <c:v>32777.659200000009</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>32700.535296000005</c:v>
+                        <c:v>34744.318752000006</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>34662.567413760007</c:v>
+                        <c:v>36828.977877120007</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>36742.321458585611</c:v>
+                        <c:v>39038.716549747209</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>38946.860746100749</c:v>
+                        <c:v>41381.03954273204</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>41283.672390866799</c:v>
+                        <c:v>43863.901915295966</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>43760.692734318807</c:v>
+                        <c:v>46495.736030213724</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>46386.334298377937</c:v>
+                        <c:v>49285.480192026545</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>49169.514356280619</c:v>
+                        <c:v>52242.609003548147</c:v>
                       </c:pt>
                       <c:pt idx="11">
-                        <c:v>52119.685217657461</c:v>
+                        <c:v>55377.165543761039</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>55246.866330716912</c:v>
+                        <c:v>58699.795476386702</c:v>
                       </c:pt>
                       <c:pt idx="13">
-                        <c:v>58561.678310559924</c:v>
+                        <c:v>62221.783204969906</c:v>
                       </c:pt>
                       <c:pt idx="14">
-                        <c:v>62075.37900919353</c:v>
+                        <c:v>65955.090197268102</c:v>
                       </c:pt>
                       <c:pt idx="15">
-                        <c:v>65799.901749745142</c:v>
+                        <c:v>69912.395609104191</c:v>
                       </c:pt>
                       <c:pt idx="16">
-                        <c:v>69747.895854729853</c:v>
+                        <c:v>74107.139345650459</c:v>
                       </c:pt>
                       <c:pt idx="17">
-                        <c:v>73932.769606013651</c:v>
+                        <c:v>78553.567706389484</c:v>
                       </c:pt>
                       <c:pt idx="18">
-                        <c:v>78368.735782374468</c:v>
+                        <c:v>83266.781768772868</c:v>
                       </c:pt>
                       <c:pt idx="19">
-                        <c:v>83070.859929316939</c:v>
+                        <c:v>88262.788674899231</c:v>
                       </c:pt>
                       <c:pt idx="20">
-                        <c:v>88055.111525075961</c:v>
+                        <c:v>93558.555995393195</c:v>
                       </c:pt>
                       <c:pt idx="21">
-                        <c:v>93338.418216580525</c:v>
+                        <c:v>99172.069355116779</c:v>
                       </c:pt>
                       <c:pt idx="22">
-                        <c:v>98938.723309575362</c:v>
+                        <c:v>105122.39351642379</c:v>
                       </c:pt>
                       <c:pt idx="23">
-                        <c:v>104875.04670814989</c:v>
+                        <c:v>111429.73712740921</c:v>
                       </c:pt>
                       <c:pt idx="24">
-                        <c:v>111167.54951063888</c:v>
+                        <c:v>118115.52135505377</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2594,10 +2593,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.1608806401931217"/>
-          <c:y val="8.0188066395467564E-2"/>
+          <c:x val="9.0169500063632127E-2"/>
+          <c:y val="8.0187995208283541E-2"/>
           <c:w val="0.27944186937285614"/>
-          <c:h val="0.24672550962497988"/>
+          <c:h val="0.14636775889866555"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2631,6 +2630,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -2638,7 +2638,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -3221,15 +3220,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>20955</xdr:colOff>
+      <xdr:colOff>11186</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>106971</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
+      <xdr:colOff>2931</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>12066</xdr:rowOff>
+      <xdr:rowOff>99987</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3576,31 +3575,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EA2527A-3BE5-4BA5-A375-284826528062}">
   <dimension ref="A1:Q62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.109375" customWidth="1"/>
-    <col min="2" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.88671875" customWidth="1"/>
-    <col min="7" max="7" width="26.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" customWidth="1"/>
+    <col min="2" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" customWidth="1"/>
+    <col min="7" max="7" width="26.1640625" style="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.33203125" style="8" customWidth="1"/>
-    <col min="9" max="9" width="14.44140625" style="8" customWidth="1"/>
+    <col min="9" max="9" width="14.5" style="8" customWidth="1"/>
     <col min="10" max="10" width="11.6640625" customWidth="1"/>
-    <col min="11" max="11" width="10.5546875" customWidth="1"/>
-    <col min="12" max="12" width="9.5546875" customWidth="1"/>
-    <col min="13" max="13" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.21875" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5" customWidth="1"/>
+    <col min="12" max="12" width="9.5" customWidth="1"/>
+    <col min="13" max="13" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.1640625" style="8" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -3615,7 +3614,7 @@
       </c>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -3630,7 +3629,7 @@
       </c>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -3641,11 +3640,11 @@
         <v>14</v>
       </c>
       <c r="E3" s="4">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -3659,12 +3658,12 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="2">
-        <v>750000</v>
+        <v>740000</v>
       </c>
       <c r="D5" t="s">
         <v>24</v>
@@ -3673,70 +3672,70 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B16" s="2"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B17" s="2"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B18" s="2"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B19" s="2"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B20" s="2"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B21" s="2"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B22" s="2"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B23" s="2"/>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B24" s="2"/>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B25" s="2"/>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B26" s="2"/>
     </row>
-    <row r="27" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
         <v>5</v>
       </c>
@@ -3783,7 +3782,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1</v>
       </c>
@@ -3805,19 +3804,19 @@
       </c>
       <c r="F28" s="3">
         <f>52*K28</f>
-        <v>27456</v>
+        <v>29172</v>
       </c>
       <c r="G28" s="8">
         <f>B28+F28+M28</f>
-        <v>-7791.2005758824362</v>
+        <v>-10244.154060705949</v>
       </c>
       <c r="H28" s="8">
         <f>Initial_Value*(1+cap_appreciation_rate)</f>
-        <v>795000</v>
+        <v>784400</v>
       </c>
       <c r="I28" s="8">
         <f>H28-E28</f>
-        <v>195927.23257588246</v>
+        <v>185327.23257588246</v>
       </c>
       <c r="J28" s="1">
         <f t="shared" ref="J28:J57" si="3">B28/52</f>
@@ -3825,24 +3824,24 @@
       </c>
       <c r="K28">
         <f>rental_income*rental_yield</f>
-        <v>528</v>
+        <v>561</v>
       </c>
       <c r="L28" s="2">
         <v>0</v>
       </c>
       <c r="M28" s="2">
-        <f t="shared" ref="M28:M57" si="4">-D28*tax_rate</f>
-        <v>6729.9920000000002</v>
+        <f>-N28*tax_rate</f>
+        <v>2561.0385151764876</v>
       </c>
       <c r="N28" s="8">
         <f>B28+F28</f>
-        <v>-14521.192575882436</v>
+        <v>-12805.192575882436</v>
       </c>
       <c r="O28" s="2"/>
       <c r="P28" s="2"/>
       <c r="Q28" s="2"/>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2</v>
       </c>
@@ -3863,45 +3862,45 @@
         <v>590284.20616353117</v>
       </c>
       <c r="F29" s="3">
-        <f t="shared" ref="F29:F57" si="5">52*K29</f>
-        <v>29103.360000000004</v>
+        <f t="shared" ref="F29:F57" si="4">52*K29</f>
+        <v>30922.320000000003</v>
       </c>
       <c r="G29" s="8">
-        <f t="shared" ref="G29:G57" si="6">B29+F29+M29</f>
-        <v>-6236.1063128232099</v>
+        <f t="shared" ref="G29:G57" si="5">B29+F29+M29</f>
+        <v>-8843.8980607059457</v>
       </c>
       <c r="H29" s="8">
-        <f t="shared" ref="H29:H57" si="7">H28*(1+cap_appreciation_rate)</f>
-        <v>842700</v>
+        <f t="shared" ref="H29:H57" si="6">H28*(1+cap_appreciation_rate)</f>
+        <v>831464</v>
       </c>
       <c r="I29" s="8">
-        <f t="shared" ref="I29:I57" si="8">H29-E29</f>
-        <v>252415.79383646883</v>
+        <f t="shared" ref="I29:I57" si="7">H29-E29</f>
+        <v>241179.79383646883</v>
       </c>
       <c r="J29" s="1">
         <f t="shared" si="3"/>
         <v>-807.2537033823545</v>
       </c>
       <c r="K29" s="9">
-        <f t="shared" ref="K29:K57" si="9">K28*(1+rental_growth)</f>
-        <v>559.68000000000006</v>
+        <f t="shared" ref="K29:K57" si="8">K28*(1+rental_growth)</f>
+        <v>594.66000000000008</v>
       </c>
       <c r="L29" s="2">
         <v>0</v>
       </c>
       <c r="M29" s="2">
-        <f t="shared" si="4"/>
-        <v>6637.7262630592222</v>
+        <f>-N29*tax_rate</f>
+        <v>2210.9745151764869</v>
       </c>
       <c r="N29" s="8">
-        <f t="shared" ref="N29:N57" si="10">B29+F29</f>
-        <v>-12873.832575882432</v>
+        <f t="shared" ref="N29:N57" si="9">B29+F29</f>
+        <v>-11054.872575882433</v>
       </c>
       <c r="O29" s="2"/>
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>3</v>
       </c>
@@ -3918,49 +3917,49 @@
         <v>-32701.745021459632</v>
       </c>
       <c r="E30" s="3">
-        <f t="shared" ref="E30:E57" si="11">E29+C30</f>
+        <f t="shared" ref="E30:E57" si="10">E29+C30</f>
         <v>581008.75860910839</v>
       </c>
       <c r="F30" s="3">
+        <f t="shared" si="4"/>
+        <v>32777.659200000009</v>
+      </c>
+      <c r="G30" s="8">
         <f t="shared" si="5"/>
-        <v>30849.561600000008</v>
-      </c>
-      <c r="G30" s="8">
+        <v>-7359.6267007059414</v>
+      </c>
+      <c r="H30" s="8">
         <f t="shared" si="6"/>
-        <v>-4587.2819715905016</v>
-      </c>
-      <c r="H30" s="8">
+        <v>881351.84000000008</v>
+      </c>
+      <c r="I30" s="8">
         <f t="shared" si="7"/>
-        <v>893262</v>
-      </c>
-      <c r="I30" s="8">
-        <f t="shared" si="8"/>
-        <v>312253.24139089161</v>
+        <v>300343.08139089169</v>
       </c>
       <c r="J30" s="1">
         <f t="shared" si="3"/>
         <v>-807.2537033823545</v>
       </c>
       <c r="K30" s="9">
-        <f t="shared" si="9"/>
-        <v>593.26080000000013</v>
+        <f t="shared" si="8"/>
+        <v>630.33960000000013</v>
       </c>
       <c r="L30" s="2">
         <v>0</v>
       </c>
       <c r="M30" s="2">
-        <f t="shared" si="4"/>
-        <v>6540.3490042919266</v>
+        <f>-N30*tax_rate</f>
+        <v>1839.9066751764856</v>
       </c>
       <c r="N30" s="8">
-        <f t="shared" si="10"/>
-        <v>-11127.630975882428</v>
+        <f t="shared" si="9"/>
+        <v>-9199.5333758824272</v>
       </c>
       <c r="O30" s="2"/>
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>4</v>
       </c>
@@ -3977,49 +3976,49 @@
         <v>-32187.885226944611</v>
       </c>
       <c r="E31" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>571219.45126017055</v>
       </c>
       <c r="F31" s="3">
+        <f t="shared" si="4"/>
+        <v>34744.318752000006</v>
+      </c>
+      <c r="G31" s="8">
         <f t="shared" si="5"/>
-        <v>32700.535296000005</v>
-      </c>
-      <c r="G31" s="8">
+        <v>-5786.2990591059443</v>
+      </c>
+      <c r="H31" s="8">
         <f t="shared" si="6"/>
-        <v>-2839.0802344935082</v>
-      </c>
-      <c r="H31" s="8">
+        <v>934232.95040000009</v>
+      </c>
+      <c r="I31" s="8">
         <f t="shared" si="7"/>
-        <v>946857.72000000009</v>
-      </c>
-      <c r="I31" s="8">
-        <f t="shared" si="8"/>
-        <v>375638.26873982954</v>
+        <v>363013.49913982954</v>
       </c>
       <c r="J31" s="1">
         <f t="shared" si="3"/>
         <v>-807.2537033823545</v>
       </c>
       <c r="K31" s="9">
-        <f t="shared" si="9"/>
-        <v>628.85644800000011</v>
+        <f t="shared" si="8"/>
+        <v>668.15997600000014</v>
       </c>
       <c r="L31" s="2">
         <v>0</v>
       </c>
       <c r="M31" s="2">
-        <f t="shared" si="4"/>
-        <v>6437.5770453889227</v>
+        <f>-N31*tax_rate</f>
+        <v>1446.5747647764861</v>
       </c>
       <c r="N31" s="8">
-        <f t="shared" si="10"/>
-        <v>-9276.6572798824309</v>
+        <f t="shared" si="9"/>
+        <v>-7232.8738238824299</v>
       </c>
       <c r="O31" s="2"/>
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>5</v>
       </c>
@@ -4036,49 +4035,49 @@
         <v>-31645.557599813459</v>
       </c>
       <c r="E32" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>560887.81628410157</v>
       </c>
       <c r="F32" s="3">
+        <f t="shared" si="4"/>
+        <v>36828.977877120007</v>
+      </c>
+      <c r="G32" s="8">
         <f t="shared" si="5"/>
-        <v>34662.567413760007</v>
-      </c>
-      <c r="G32" s="8">
+        <v>-4118.571759009943</v>
+      </c>
+      <c r="H32" s="8">
         <f t="shared" si="6"/>
-        <v>-985.51364215973717</v>
-      </c>
-      <c r="H32" s="8">
+        <v>990286.92742400011</v>
+      </c>
+      <c r="I32" s="8">
         <f t="shared" si="7"/>
-        <v>1003669.1832000001</v>
-      </c>
-      <c r="I32" s="8">
-        <f t="shared" si="8"/>
-        <v>442781.36691589851</v>
+        <v>429399.11113989854</v>
       </c>
       <c r="J32" s="1">
         <f t="shared" si="3"/>
         <v>-807.2537033823545</v>
       </c>
       <c r="K32" s="9">
-        <f t="shared" si="9"/>
-        <v>666.58783488000017</v>
+        <f t="shared" si="8"/>
+        <v>708.24957456000016</v>
       </c>
       <c r="L32" s="2">
         <v>0</v>
       </c>
       <c r="M32" s="2">
-        <f t="shared" si="4"/>
-        <v>6329.111519962692</v>
+        <f>-N32*tax_rate</f>
+        <v>1029.642939752486</v>
       </c>
       <c r="N32" s="8">
-        <f t="shared" si="10"/>
-        <v>-7314.6251621224292</v>
+        <f t="shared" si="9"/>
+        <v>-5148.2146987624292</v>
       </c>
       <c r="O32" s="2"/>
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>6</v>
       </c>
@@ -4095,49 +4094,49 @@
         <v>-31073.185022139231</v>
       </c>
       <c r="E33" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>549983.80873035837</v>
       </c>
       <c r="F33" s="3">
+        <f t="shared" si="4"/>
+        <v>39038.716549747209</v>
+      </c>
+      <c r="G33" s="8">
         <f t="shared" si="5"/>
-        <v>36742.321458585611</v>
-      </c>
-      <c r="G33" s="8">
+        <v>-2350.7808209081822</v>
+      </c>
+      <c r="H33" s="8">
         <f t="shared" si="6"/>
-        <v>979.76588713102137</v>
-      </c>
-      <c r="H33" s="8">
+        <v>1049704.1430694403</v>
+      </c>
+      <c r="I33" s="8">
         <f t="shared" si="7"/>
-        <v>1063889.3341920001</v>
-      </c>
-      <c r="I33" s="8">
-        <f t="shared" si="8"/>
-        <v>513905.52546164172</v>
+        <v>499720.33433908189</v>
       </c>
       <c r="J33" s="1">
         <f t="shared" si="3"/>
         <v>-807.2537033823545</v>
       </c>
       <c r="K33" s="9">
-        <f t="shared" si="9"/>
-        <v>706.58310497280024</v>
+        <f t="shared" si="8"/>
+        <v>750.74454903360015</v>
       </c>
       <c r="L33" s="2">
         <v>0</v>
       </c>
       <c r="M33" s="2">
-        <f t="shared" si="4"/>
-        <v>6214.6370044278465</v>
+        <f>-N33*tax_rate</f>
+        <v>587.69520522704556</v>
       </c>
       <c r="N33" s="8">
-        <f t="shared" si="10"/>
-        <v>-5234.8711172968251</v>
+        <f t="shared" si="9"/>
+        <v>-2938.4760261352276</v>
       </c>
       <c r="O33" s="2"/>
       <c r="P33" s="2"/>
       <c r="Q33" s="2"/>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>7</v>
       </c>
@@ -4154,49 +4153,49 @@
         <v>-30469.103003661865</v>
       </c>
       <c r="E34" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>538475.7191581378</v>
       </c>
       <c r="F34" s="3">
+        <f t="shared" si="4"/>
+        <v>41381.03954273204</v>
+      </c>
+      <c r="G34" s="8">
         <f t="shared" si="5"/>
-        <v>38946.860746100749</v>
-      </c>
-      <c r="G34" s="8">
+        <v>-476.92242652031712</v>
+      </c>
+      <c r="H34" s="8">
         <f t="shared" si="6"/>
-        <v>3063.4887709506856</v>
-      </c>
-      <c r="H34" s="8">
+        <v>1112686.3916536067</v>
+      </c>
+      <c r="I34" s="8">
         <f t="shared" si="7"/>
-        <v>1127722.6942435203</v>
-      </c>
-      <c r="I34" s="8">
-        <f t="shared" si="8"/>
-        <v>589246.97508538247</v>
+        <v>574210.67249546887</v>
       </c>
       <c r="J34" s="1">
         <f t="shared" si="3"/>
         <v>-807.2537033823545</v>
       </c>
       <c r="K34" s="9">
-        <f t="shared" si="9"/>
-        <v>748.9780912711683</v>
+        <f t="shared" si="8"/>
+        <v>795.78922197561621</v>
       </c>
       <c r="L34" s="2">
         <v>0</v>
       </c>
       <c r="M34" s="2">
-        <f t="shared" si="4"/>
-        <v>6093.8206007323734</v>
+        <f>-N34*tax_rate</f>
+        <v>119.23060663007928</v>
       </c>
       <c r="N34" s="8">
-        <f t="shared" si="10"/>
-        <v>-3030.3318297816877</v>
+        <f t="shared" si="9"/>
+        <v>-596.15303315039637</v>
       </c>
       <c r="O34" s="2"/>
       <c r="P34" s="2"/>
       <c r="Q34" s="2"/>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>8</v>
       </c>
@@ -4213,49 +4212,49 @@
         <v>-29831.554841360845</v>
       </c>
       <c r="E35" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>526330.08142361615</v>
       </c>
       <c r="F35" s="3">
+        <f t="shared" si="4"/>
+        <v>43863.901915295966</v>
+      </c>
+      <c r="G35" s="8">
         <f t="shared" si="5"/>
-        <v>41283.672390866799</v>
-      </c>
-      <c r="G35" s="8">
+        <v>1509.3674715308239</v>
+      </c>
+      <c r="H35" s="8">
         <f t="shared" si="6"/>
-        <v>5272.7907832565324</v>
-      </c>
-      <c r="H35" s="8">
+        <v>1179447.5751528232</v>
+      </c>
+      <c r="I35" s="8">
         <f t="shared" si="7"/>
-        <v>1195386.0558981316</v>
-      </c>
-      <c r="I35" s="8">
-        <f t="shared" si="8"/>
-        <v>669055.97447451542</v>
+        <v>653117.49372920708</v>
       </c>
       <c r="J35" s="1">
         <f t="shared" si="3"/>
         <v>-807.2537033823545</v>
       </c>
       <c r="K35" s="9">
-        <f t="shared" si="9"/>
-        <v>793.91677674743846</v>
+        <f t="shared" si="8"/>
+        <v>843.53657529415318</v>
       </c>
       <c r="L35" s="2">
         <v>0</v>
       </c>
       <c r="M35" s="2">
-        <f t="shared" si="4"/>
-        <v>5966.3109682721697</v>
+        <f>-N35*tax_rate</f>
+        <v>-377.34186788270603</v>
       </c>
       <c r="N35" s="8">
-        <f t="shared" si="10"/>
-        <v>-693.52018501563725</v>
+        <f t="shared" si="9"/>
+        <v>1886.70933941353</v>
       </c>
       <c r="O35" s="2"/>
       <c r="P35" s="2"/>
       <c r="Q35" s="2"/>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>9</v>
       </c>
@@ -4272,49 +4271,49 @@
         <v>-29158.686510868345</v>
       </c>
       <c r="E36" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>513511.57535860204</v>
       </c>
       <c r="F36" s="3">
+        <f t="shared" si="4"/>
+        <v>46495.736030213724</v>
+      </c>
+      <c r="G36" s="8">
         <f t="shared" si="5"/>
-        <v>43760.692734318807</v>
-      </c>
-      <c r="G36" s="8">
+        <v>3614.8347634650299</v>
+      </c>
+      <c r="H36" s="8">
         <f t="shared" si="6"/>
-        <v>7615.2374606100402</v>
-      </c>
-      <c r="H36" s="8">
+        <v>1250214.4296619927</v>
+      </c>
+      <c r="I36" s="8">
         <f t="shared" si="7"/>
-        <v>1267109.2192520194</v>
-      </c>
-      <c r="I36" s="8">
-        <f t="shared" si="8"/>
-        <v>753597.64389341744</v>
+        <v>736702.85430339072</v>
       </c>
       <c r="J36" s="1">
         <f t="shared" si="3"/>
         <v>-807.2537033823545</v>
       </c>
       <c r="K36" s="9">
-        <f t="shared" si="9"/>
-        <v>841.55178335228482</v>
+        <f t="shared" si="8"/>
+        <v>894.14876981180237</v>
       </c>
       <c r="L36" s="2">
         <v>0</v>
       </c>
       <c r="M36" s="2">
-        <f t="shared" si="4"/>
-        <v>5831.7373021736694</v>
+        <f>-N36*tax_rate</f>
+        <v>-903.7086908662576</v>
       </c>
       <c r="N36" s="8">
-        <f t="shared" si="10"/>
-        <v>1783.5001584363708</v>
+        <f t="shared" si="9"/>
+        <v>4518.5434543312876</v>
       </c>
       <c r="O36" s="2"/>
       <c r="P36" s="2"/>
       <c r="Q36" s="2"/>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>10</v>
       </c>
@@ -4331,49 +4330,49 @@
         <v>-28448.541274866566</v>
       </c>
       <c r="E37" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>499982.92405758618</v>
       </c>
       <c r="F37" s="3">
+        <f t="shared" si="4"/>
+        <v>49285.480192026545</v>
+      </c>
+      <c r="G37" s="8">
         <f t="shared" si="5"/>
-        <v>46386.334298377937</v>
-      </c>
-      <c r="G37" s="8">
+        <v>5846.6300929152876</v>
+      </c>
+      <c r="H37" s="8">
         <f t="shared" si="6"/>
-        <v>10098.849977468813</v>
-      </c>
-      <c r="H37" s="8">
+        <v>1325227.2954417123</v>
+      </c>
+      <c r="I37" s="8">
         <f t="shared" si="7"/>
-        <v>1343135.7724071406</v>
-      </c>
-      <c r="I37" s="8">
-        <f t="shared" si="8"/>
-        <v>843152.84834955446</v>
+        <v>825244.37138412613</v>
       </c>
       <c r="J37" s="1">
         <f t="shared" si="3"/>
         <v>-807.2537033823545</v>
       </c>
       <c r="K37" s="9">
-        <f t="shared" si="9"/>
-        <v>892.04489035342192</v>
+        <f t="shared" si="8"/>
+        <v>947.79769600051054</v>
       </c>
       <c r="L37" s="2">
         <v>0</v>
       </c>
       <c r="M37" s="2">
-        <f t="shared" si="4"/>
-        <v>5689.7082549733132</v>
+        <f>-N37*tax_rate</f>
+        <v>-1461.6575232288219</v>
       </c>
       <c r="N37" s="8">
-        <f t="shared" si="10"/>
-        <v>4409.1417224955003</v>
+        <f t="shared" si="9"/>
+        <v>7308.2876161441091</v>
       </c>
       <c r="O37" s="2"/>
       <c r="P37" s="2"/>
       <c r="Q37" s="2"/>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>11</v>
       </c>
@@ -4390,49 +4389,49 @@
         <v>-27699.053992790283</v>
       </c>
       <c r="E38" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>485704.78547449404</v>
       </c>
       <c r="F38" s="3">
+        <f t="shared" si="4"/>
+        <v>52242.609003548147</v>
+      </c>
+      <c r="G38" s="8">
         <f t="shared" si="5"/>
-        <v>49169.514356280619</v>
-      </c>
-      <c r="G38" s="8">
+        <v>8212.3331421325674</v>
+      </c>
+      <c r="H38" s="8">
         <f t="shared" si="6"/>
-        <v>12732.13257895624</v>
-      </c>
-      <c r="H38" s="8">
+        <v>1404740.933168215</v>
+      </c>
+      <c r="I38" s="8">
         <f t="shared" si="7"/>
-        <v>1423723.918751569</v>
-      </c>
-      <c r="I38" s="8">
-        <f t="shared" si="8"/>
-        <v>938019.1332770749</v>
+        <v>919036.14769372088</v>
       </c>
       <c r="J38" s="1">
         <f t="shared" si="3"/>
         <v>-807.2537033823545</v>
       </c>
       <c r="K38" s="9">
-        <f t="shared" si="9"/>
-        <v>945.56758377462734</v>
+        <f t="shared" si="8"/>
+        <v>1004.6655577605412</v>
       </c>
       <c r="L38" s="2">
         <v>0</v>
       </c>
       <c r="M38" s="2">
-        <f t="shared" si="4"/>
-        <v>5539.8107985580573</v>
+        <f>-N38*tax_rate</f>
+        <v>-2053.0832855331423</v>
       </c>
       <c r="N38" s="8">
-        <f t="shared" si="10"/>
-        <v>7192.3217803981825</v>
+        <f t="shared" si="9"/>
+        <v>10265.41642766571</v>
       </c>
       <c r="O38" s="2"/>
       <c r="P38" s="2"/>
       <c r="Q38" s="2"/>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>12</v>
       </c>
@@ -4449,49 +4448,49 @@
         <v>-26908.045115286979</v>
       </c>
       <c r="E39" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>470635.63801389857</v>
       </c>
       <c r="F39" s="3">
+        <f t="shared" si="4"/>
+        <v>55377.165543761039</v>
+      </c>
+      <c r="G39" s="8">
         <f t="shared" si="5"/>
-        <v>52119.685217657461</v>
-      </c>
-      <c r="G39" s="8">
+        <v>10719.978374302882</v>
+      </c>
+      <c r="H39" s="8">
         <f t="shared" si="6"/>
-        <v>15524.101664832422</v>
-      </c>
-      <c r="H39" s="8">
+        <v>1489025.389158308</v>
+      </c>
+      <c r="I39" s="8">
         <f t="shared" si="7"/>
-        <v>1509147.3538766631</v>
-      </c>
-      <c r="I39" s="8">
-        <f t="shared" si="8"/>
-        <v>1038511.7158627645</v>
+        <v>1018389.7511444094</v>
       </c>
       <c r="J39" s="1">
         <f t="shared" si="3"/>
         <v>-807.2537033823545</v>
       </c>
       <c r="K39" s="9">
-        <f t="shared" si="9"/>
-        <v>1002.301638801105</v>
+        <f t="shared" si="8"/>
+        <v>1064.9454912261738</v>
       </c>
       <c r="L39" s="2">
         <v>0</v>
       </c>
       <c r="M39" s="2">
-        <f t="shared" si="4"/>
-        <v>5381.6090230573964</v>
+        <f>-N39*tax_rate</f>
+        <v>-2679.9945935757205</v>
       </c>
       <c r="N39" s="8">
-        <f t="shared" si="10"/>
-        <v>10142.492641775025</v>
+        <f t="shared" si="9"/>
+        <v>13399.972967878603</v>
       </c>
       <c r="O39" s="2"/>
       <c r="P39" s="2"/>
       <c r="Q39" s="2"/>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>13</v>
       </c>
@@ -4508,49 +4507,49 @@
         <v>-26073.214345969995</v>
       </c>
       <c r="E40" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>454731.65978398611</v>
       </c>
       <c r="F40" s="3">
+        <f t="shared" si="4"/>
+        <v>58699.795476386702</v>
+      </c>
+      <c r="G40" s="8">
         <f t="shared" si="5"/>
-        <v>55246.866330716912</v>
-      </c>
-      <c r="G40" s="8">
+        <v>13378.082320403413</v>
+      </c>
+      <c r="H40" s="8">
         <f t="shared" si="6"/>
-        <v>18484.316624028474</v>
-      </c>
-      <c r="H40" s="8">
+        <v>1578366.9125078067</v>
+      </c>
+      <c r="I40" s="8">
         <f t="shared" si="7"/>
-        <v>1599696.1951092631</v>
-      </c>
-      <c r="I40" s="8">
-        <f t="shared" si="8"/>
-        <v>1144964.5353252769</v>
+        <v>1123635.2527238205</v>
       </c>
       <c r="J40" s="1">
         <f t="shared" si="3"/>
         <v>-807.2537033823545</v>
       </c>
       <c r="K40" s="9">
-        <f t="shared" si="9"/>
-        <v>1062.4397371291714</v>
+        <f t="shared" si="8"/>
+        <v>1128.8422206997443</v>
       </c>
       <c r="L40" s="2">
         <v>0</v>
       </c>
       <c r="M40" s="2">
-        <f t="shared" si="4"/>
-        <v>5214.6428691939991</v>
+        <f>-N40*tax_rate</f>
+        <v>-3344.5205801008533</v>
       </c>
       <c r="N40" s="8">
-        <f t="shared" si="10"/>
-        <v>13269.673754834475</v>
+        <f t="shared" si="9"/>
+        <v>16722.602900504266</v>
       </c>
       <c r="O40" s="2"/>
       <c r="P40" s="2"/>
       <c r="Q40" s="2"/>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>14</v>
       </c>
@@ -4567,49 +4566,49 @@
         <v>-25192.133952032844</v>
       </c>
       <c r="E41" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>437946.60116013652</v>
       </c>
       <c r="F41" s="3">
+        <f t="shared" si="4"/>
+        <v>62221.783204969906</v>
+      </c>
+      <c r="G41" s="8">
         <f t="shared" si="5"/>
-        <v>58561.678310559924</v>
-      </c>
-      <c r="G41" s="8">
+        <v>16195.672503269976</v>
+      </c>
+      <c r="H41" s="8">
         <f t="shared" si="6"/>
-        <v>21622.912525084059</v>
-      </c>
-      <c r="H41" s="8">
+        <v>1673068.9272582752</v>
+      </c>
+      <c r="I41" s="8">
         <f t="shared" si="7"/>
-        <v>1695677.966815819</v>
-      </c>
-      <c r="I41" s="8">
-        <f t="shared" si="8"/>
-        <v>1257731.3656556825</v>
+        <v>1235122.3260981387</v>
       </c>
       <c r="J41" s="1">
         <f t="shared" si="3"/>
         <v>-807.2537033823545</v>
       </c>
       <c r="K41" s="9">
-        <f t="shared" si="9"/>
-        <v>1126.1861213569216</v>
+        <f t="shared" si="8"/>
+        <v>1196.5727539417289</v>
       </c>
       <c r="L41" s="2">
         <v>0</v>
       </c>
       <c r="M41" s="2">
-        <f t="shared" si="4"/>
-        <v>5038.4267904065691</v>
+        <f>-N41*tax_rate</f>
+        <v>-4048.918125817494</v>
       </c>
       <c r="N41" s="8">
-        <f t="shared" si="10"/>
-        <v>16584.485734677488</v>
+        <f t="shared" si="9"/>
+        <v>20244.59062908747</v>
       </c>
       <c r="O41" s="2"/>
       <c r="P41" s="2"/>
       <c r="Q41" s="2"/>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>15</v>
       </c>
@@ -4626,49 +4625,49 @@
         <v>-24262.241704271575</v>
       </c>
       <c r="E42" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>420231.65028852568</v>
       </c>
       <c r="F42" s="3">
+        <f t="shared" si="4"/>
+        <v>65955.090197268102</v>
+      </c>
+      <c r="G42" s="8">
         <f t="shared" si="5"/>
-        <v>62075.37900919353</v>
-      </c>
-      <c r="G42" s="8">
+        <v>19182.318097108531</v>
+      </c>
+      <c r="H42" s="8">
         <f t="shared" si="6"/>
-        <v>24950.63477416541</v>
-      </c>
-      <c r="H42" s="8">
+        <v>1773453.0628937718</v>
+      </c>
+      <c r="I42" s="8">
         <f t="shared" si="7"/>
-        <v>1797418.6448247682</v>
-      </c>
-      <c r="I42" s="8">
-        <f t="shared" si="8"/>
-        <v>1377186.9945362424</v>
+        <v>1353221.4126052461</v>
       </c>
       <c r="J42" s="1">
         <f t="shared" si="3"/>
         <v>-807.2537033823545</v>
       </c>
       <c r="K42" s="9">
-        <f t="shared" si="9"/>
-        <v>1193.7572886383371</v>
+        <f t="shared" si="8"/>
+        <v>1268.3671191782328</v>
       </c>
       <c r="L42" s="2">
         <v>0</v>
       </c>
       <c r="M42" s="2">
-        <f t="shared" si="4"/>
-        <v>4852.4483408543156</v>
+        <f>-N42*tax_rate</f>
+        <v>-4795.5795242771337</v>
       </c>
       <c r="N42" s="8">
-        <f t="shared" si="10"/>
-        <v>20098.186433311093</v>
+        <f t="shared" si="9"/>
+        <v>23977.897621385666</v>
       </c>
       <c r="O42" s="2"/>
       <c r="P42" s="2"/>
       <c r="Q42" s="2"/>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>16</v>
       </c>
@@ -4685,49 +4684,49 @@
         <v>-23280.833425984336</v>
       </c>
       <c r="E43" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>401535.29113862757</v>
       </c>
       <c r="F43" s="3">
+        <f t="shared" si="4"/>
+        <v>69912.395609104191</v>
+      </c>
+      <c r="G43" s="8">
         <f t="shared" si="5"/>
-        <v>65799.901749745142</v>
-      </c>
-      <c r="G43" s="8">
+        <v>22348.162426577404</v>
+      </c>
+      <c r="H43" s="8">
         <f t="shared" si="6"/>
-        <v>28478.875859059575</v>
-      </c>
-      <c r="H43" s="8">
+        <v>1879860.2466673981</v>
+      </c>
+      <c r="I43" s="8">
         <f t="shared" si="7"/>
-        <v>1905263.7635142545</v>
-      </c>
-      <c r="I43" s="8">
-        <f t="shared" si="8"/>
-        <v>1503728.4723756269</v>
+        <v>1478324.9555287706</v>
       </c>
       <c r="J43" s="1">
         <f t="shared" si="3"/>
         <v>-807.2537033823545</v>
       </c>
       <c r="K43" s="9">
-        <f t="shared" si="9"/>
-        <v>1265.3827259566374</v>
+        <f t="shared" si="8"/>
+        <v>1344.4691463289269</v>
       </c>
       <c r="L43" s="2">
         <v>0</v>
       </c>
       <c r="M43" s="2">
-        <f t="shared" si="4"/>
-        <v>4656.1666851968675</v>
+        <f>-N43*tax_rate</f>
+        <v>-5587.0406066443511</v>
       </c>
       <c r="N43" s="8">
-        <f t="shared" si="10"/>
-        <v>23822.709173862706</v>
+        <f t="shared" si="9"/>
+        <v>27935.203033221755</v>
       </c>
       <c r="O43" s="2"/>
       <c r="P43" s="2"/>
       <c r="Q43" s="2"/>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>17</v>
       </c>
@@ -4744,49 +4743,49 @@
         <v>-22245.055129079978</v>
       </c>
       <c r="E44" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>381803.15369182511</v>
       </c>
       <c r="F44" s="3">
+        <f t="shared" si="4"/>
+        <v>74107.139345650459</v>
+      </c>
+      <c r="G44" s="8">
         <f t="shared" si="5"/>
-        <v>69747.895854729853</v>
-      </c>
-      <c r="G44" s="8">
+        <v>25703.957415814417</v>
+      </c>
+      <c r="H44" s="8">
         <f t="shared" si="6"/>
-        <v>32219.714304663412</v>
-      </c>
-      <c r="H44" s="8">
+        <v>1992651.8614674422</v>
+      </c>
+      <c r="I44" s="8">
         <f t="shared" si="7"/>
-        <v>2019579.5893251097</v>
-      </c>
-      <c r="I44" s="8">
-        <f t="shared" si="8"/>
-        <v>1637776.4356332845</v>
+        <v>1610848.707775617</v>
       </c>
       <c r="J44" s="1">
         <f t="shared" si="3"/>
         <v>-807.2537033823545</v>
       </c>
       <c r="K44" s="9">
-        <f t="shared" si="9"/>
-        <v>1341.3056895140357</v>
+        <f t="shared" si="8"/>
+        <v>1425.1372951086626</v>
       </c>
       <c r="L44" s="2">
         <v>0</v>
       </c>
       <c r="M44" s="2">
-        <f t="shared" si="4"/>
-        <v>4449.0110258159957</v>
+        <f>-N44*tax_rate</f>
+        <v>-6425.9893539536051</v>
       </c>
       <c r="N44" s="8">
-        <f t="shared" si="10"/>
-        <v>27770.703278847417</v>
+        <f t="shared" si="9"/>
+        <v>32129.946769768023</v>
       </c>
       <c r="O44" s="2"/>
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>18</v>
       </c>
@@ -4803,49 +4802,49 @@
         <v>-21151.894714527127</v>
       </c>
       <c r="E45" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>360977.85583046981</v>
       </c>
       <c r="F45" s="3">
+        <f t="shared" si="4"/>
+        <v>78553.567706389484</v>
+      </c>
+      <c r="G45" s="8">
         <f t="shared" si="5"/>
-        <v>73932.769606013651</v>
-      </c>
-      <c r="G45" s="8">
+        <v>29261.100104405639</v>
+      </c>
+      <c r="H45" s="8">
         <f t="shared" si="6"/>
-        <v>36185.955973036638</v>
-      </c>
-      <c r="H45" s="8">
+        <v>2112210.9731554887</v>
+      </c>
+      <c r="I45" s="8">
         <f t="shared" si="7"/>
-        <v>2140754.3646846162</v>
-      </c>
-      <c r="I45" s="8">
-        <f t="shared" si="8"/>
-        <v>1779776.5088541463</v>
+        <v>1751233.1173250189</v>
       </c>
       <c r="J45" s="1">
         <f t="shared" si="3"/>
         <v>-807.2537033823545</v>
       </c>
       <c r="K45" s="9">
-        <f t="shared" si="9"/>
-        <v>1421.7840308848779</v>
+        <f t="shared" si="8"/>
+        <v>1510.6455328151824</v>
       </c>
       <c r="L45" s="2">
         <v>0</v>
       </c>
       <c r="M45" s="2">
-        <f t="shared" si="4"/>
-        <v>4230.3789429054259</v>
+        <f>-N45*tax_rate</f>
+        <v>-7315.2750261014098</v>
       </c>
       <c r="N45" s="8">
-        <f t="shared" si="10"/>
-        <v>31955.577030131215</v>
+        <f t="shared" si="9"/>
+        <v>36576.375130507047</v>
       </c>
       <c r="O45" s="2"/>
       <c r="P45" s="2"/>
       <c r="Q45" s="2"/>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>19</v>
       </c>
@@ -4862,49 +4861,49 @@
         <v>-19998.173213008042</v>
       </c>
       <c r="E46" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>338998.83646759542</v>
       </c>
       <c r="F46" s="3">
+        <f t="shared" si="4"/>
+        <v>83266.781768772868</v>
+      </c>
+      <c r="G46" s="8">
         <f t="shared" si="5"/>
-        <v>78368.735782374468</v>
-      </c>
-      <c r="G46" s="8">
+        <v>33031.671354312348</v>
+      </c>
+      <c r="H46" s="8">
         <f t="shared" si="6"/>
-        <v>40391.177849093641</v>
-      </c>
-      <c r="H46" s="8">
+        <v>2238943.6315448182</v>
+      </c>
+      <c r="I46" s="8">
         <f t="shared" si="7"/>
-        <v>2269199.6265656934</v>
-      </c>
-      <c r="I46" s="8">
-        <f t="shared" si="8"/>
-        <v>1930200.7900980981</v>
+        <v>1899944.7950772229</v>
       </c>
       <c r="J46" s="1">
         <f t="shared" si="3"/>
         <v>-807.2537033823545</v>
       </c>
       <c r="K46" s="9">
-        <f t="shared" si="9"/>
-        <v>1507.0910727379705</v>
+        <f t="shared" si="8"/>
+        <v>1601.2842647840935</v>
       </c>
       <c r="L46" s="2">
         <v>0</v>
       </c>
       <c r="M46" s="2">
-        <f t="shared" si="4"/>
-        <v>3999.6346426016084</v>
+        <f>-N46*tax_rate</f>
+        <v>-8257.917838578087</v>
       </c>
       <c r="N46" s="8">
-        <f t="shared" si="10"/>
-        <v>36391.543206492031</v>
+        <f t="shared" si="9"/>
+        <v>41289.589192890431</v>
       </c>
       <c r="O46" s="2"/>
       <c r="P46" s="2"/>
       <c r="Q46" s="2"/>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>20</v>
       </c>
@@ -4921,49 +4920,49 @@
         <v>-18780.535540304802</v>
       </c>
       <c r="E47" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>315802.17943201779</v>
       </c>
       <c r="F47" s="3">
+        <f t="shared" si="4"/>
+        <v>88262.788674899231</v>
+      </c>
+      <c r="G47" s="8">
         <f t="shared" si="5"/>
-        <v>83070.859929316939</v>
-      </c>
-      <c r="G47" s="8">
+        <v>37028.476879213435</v>
+      </c>
+      <c r="H47" s="8">
         <f t="shared" si="6"/>
-        <v>44849.774461495464</v>
-      </c>
-      <c r="H47" s="8">
+        <v>2373280.2494375072</v>
+      </c>
+      <c r="I47" s="8">
         <f t="shared" si="7"/>
-        <v>2405351.604159635</v>
-      </c>
-      <c r="I47" s="8">
-        <f t="shared" si="8"/>
-        <v>2089549.4247276173</v>
+        <v>2057478.0700054895</v>
       </c>
       <c r="J47" s="1">
         <f t="shared" si="3"/>
         <v>-807.2537033823545</v>
       </c>
       <c r="K47" s="9">
-        <f t="shared" si="9"/>
-        <v>1597.5165371022488</v>
+        <f t="shared" si="8"/>
+        <v>1697.3613206711391</v>
       </c>
       <c r="L47" s="2">
         <v>0</v>
       </c>
       <c r="M47" s="2">
-        <f t="shared" si="4"/>
-        <v>3756.1071080609604</v>
+        <f>-N47*tax_rate</f>
+        <v>-9257.1192198033586</v>
       </c>
       <c r="N47" s="8">
-        <f t="shared" si="10"/>
-        <v>41093.667353434503</v>
+        <f t="shared" si="9"/>
+        <v>46285.596099016795</v>
       </c>
       <c r="O47" s="2"/>
       <c r="P47" s="2"/>
       <c r="Q47" s="2"/>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>21</v>
       </c>
@@ -4980,49 +4979,49 @@
         <v>-17495.440740533802</v>
       </c>
       <c r="E48" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>291320.42759666918</v>
       </c>
       <c r="F48" s="3">
+        <f t="shared" si="4"/>
+        <v>93558.555995393195</v>
+      </c>
+      <c r="G48" s="8">
         <f t="shared" si="5"/>
-        <v>88055.111525075961</v>
-      </c>
-      <c r="G48" s="8">
+        <v>41265.09073560861</v>
+      </c>
+      <c r="H48" s="8">
         <f t="shared" si="6"/>
-        <v>49577.007097300288</v>
-      </c>
-      <c r="H48" s="8">
+        <v>2515677.0644037579</v>
+      </c>
+      <c r="I48" s="8">
         <f t="shared" si="7"/>
-        <v>2549672.7004092131</v>
-      </c>
-      <c r="I48" s="8">
-        <f t="shared" si="8"/>
-        <v>2258352.2728125439</v>
+        <v>2224356.6368070887</v>
       </c>
       <c r="J48" s="1">
         <f t="shared" si="3"/>
         <v>-807.2537033823545</v>
       </c>
       <c r="K48" s="9">
-        <f t="shared" si="9"/>
-        <v>1693.3675293283839</v>
+        <f t="shared" si="8"/>
+        <v>1799.2029999114075</v>
       </c>
       <c r="L48" s="2">
         <v>0</v>
       </c>
       <c r="M48" s="2">
-        <f t="shared" si="4"/>
-        <v>3499.0881481067609</v>
+        <f>-N48*tax_rate</f>
+        <v>-10316.272683902152</v>
       </c>
       <c r="N48" s="8">
-        <f t="shared" si="10"/>
-        <v>46077.918949193525</v>
+        <f t="shared" si="9"/>
+        <v>51581.363419510759</v>
       </c>
       <c r="O48" s="2"/>
       <c r="P48" s="2"/>
       <c r="Q48" s="2"/>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>22</v>
       </c>
@@ -5039,49 +5038,49 @@
         <v>-16139.151688855485</v>
       </c>
       <c r="E49" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>265482.38670964225</v>
       </c>
       <c r="F49" s="3">
+        <f t="shared" si="4"/>
+        <v>99172.069355116779</v>
+      </c>
+      <c r="G49" s="8">
         <f t="shared" si="5"/>
-        <v>93338.418216580525</v>
-      </c>
-      <c r="G49" s="8">
+        <v>45755.901423387477</v>
+      </c>
+      <c r="H49" s="8">
         <f t="shared" si="6"/>
-        <v>54589.055978469187</v>
-      </c>
-      <c r="H49" s="8">
+        <v>2666617.6882679835</v>
+      </c>
+      <c r="I49" s="8">
         <f t="shared" si="7"/>
-        <v>2702653.0624337662</v>
-      </c>
-      <c r="I49" s="8">
-        <f t="shared" si="8"/>
-        <v>2437170.6757241241</v>
+        <v>2401135.3015583414</v>
       </c>
       <c r="J49" s="1">
         <f t="shared" si="3"/>
         <v>-807.2537033823545</v>
       </c>
       <c r="K49" s="9">
-        <f t="shared" si="9"/>
-        <v>1794.9695810880869</v>
+        <f t="shared" si="8"/>
+        <v>1907.1551799060919</v>
       </c>
       <c r="L49" s="2">
         <v>0</v>
       </c>
       <c r="M49" s="2">
-        <f t="shared" si="4"/>
-        <v>3227.8303377710972</v>
+        <f>-N49*tax_rate</f>
+        <v>-11438.975355846869</v>
       </c>
       <c r="N49" s="8">
-        <f t="shared" si="10"/>
-        <v>51361.225640698089</v>
+        <f t="shared" si="9"/>
+        <v>57194.876779234342</v>
       </c>
       <c r="O49" s="2"/>
       <c r="P49" s="2"/>
       <c r="Q49" s="2"/>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>23</v>
       </c>
@@ -5098,49 +5097,49 @@
         <v>-14707.724223714193</v>
       </c>
       <c r="E50" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>238212.918357474</v>
       </c>
       <c r="F50" s="3">
+        <f t="shared" si="4"/>
+        <v>105122.39351642379</v>
+      </c>
+      <c r="G50" s="8">
         <f t="shared" si="5"/>
-        <v>98938.723309575362</v>
-      </c>
-      <c r="G50" s="8">
+        <v>50516.160752433083</v>
+      </c>
+      <c r="H50" s="8">
         <f t="shared" si="6"/>
-        <v>59903.075578435761</v>
-      </c>
-      <c r="H50" s="8">
+        <v>2826614.7495640628</v>
+      </c>
+      <c r="I50" s="8">
         <f t="shared" si="7"/>
-        <v>2864812.2461797921</v>
-      </c>
-      <c r="I50" s="8">
-        <f t="shared" si="8"/>
-        <v>2626599.3278223183</v>
+        <v>2588401.831206589</v>
       </c>
       <c r="J50" s="1">
         <f t="shared" si="3"/>
         <v>-807.2537033823545</v>
       </c>
       <c r="K50" s="9">
-        <f t="shared" si="9"/>
-        <v>1902.6677559533723</v>
+        <f t="shared" si="8"/>
+        <v>2021.5844907004575</v>
       </c>
       <c r="L50" s="2">
         <v>0</v>
       </c>
       <c r="M50" s="2">
-        <f t="shared" si="4"/>
-        <v>2941.5448447428389</v>
+        <f>-N50*tax_rate</f>
+        <v>-12629.040188108273</v>
       </c>
       <c r="N50" s="8">
-        <f t="shared" si="10"/>
-        <v>56961.530733692925</v>
+        <f t="shared" si="9"/>
+        <v>63145.200940541356</v>
       </c>
       <c r="O50" s="2"/>
       <c r="P50" s="2"/>
       <c r="Q50" s="2"/>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>24</v>
       </c>
@@ -5157,49 +5156,49 @@
         <v>-13196.99567700407</v>
       </c>
       <c r="E51" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>209432.72145859565</v>
       </c>
       <c r="F51" s="3">
+        <f t="shared" si="4"/>
+        <v>111429.73712740921</v>
+      </c>
+      <c r="G51" s="8">
         <f t="shared" si="5"/>
-        <v>104875.04670814989</v>
-      </c>
-      <c r="G51" s="8">
+        <v>55562.035641221424</v>
+      </c>
+      <c r="H51" s="8">
         <f t="shared" si="6"/>
-        <v>65537.253267668275</v>
-      </c>
-      <c r="H51" s="8">
+        <v>2996211.6345379069</v>
+      </c>
+      <c r="I51" s="8">
         <f t="shared" si="7"/>
-        <v>3036700.98095058</v>
-      </c>
-      <c r="I51" s="8">
-        <f t="shared" si="8"/>
-        <v>2827268.2594919843</v>
+        <v>2786778.9130793111</v>
       </c>
       <c r="J51" s="1">
         <f t="shared" si="3"/>
         <v>-807.2537033823545</v>
       </c>
       <c r="K51" s="9">
-        <f t="shared" si="9"/>
-        <v>2016.8278213105748</v>
+        <f t="shared" si="8"/>
+        <v>2142.8795601424849</v>
       </c>
       <c r="L51" s="2">
         <v>0</v>
       </c>
       <c r="M51" s="2">
-        <f t="shared" si="4"/>
-        <v>2639.399135400814</v>
+        <f>-N51*tax_rate</f>
+        <v>-13890.508910305356</v>
       </c>
       <c r="N51" s="8">
-        <f t="shared" si="10"/>
-        <v>62897.854132267457</v>
+        <f t="shared" si="9"/>
+        <v>69452.544551526778</v>
       </c>
       <c r="O51" s="2"/>
       <c r="P51" s="2"/>
       <c r="Q51" s="2"/>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>25</v>
       </c>
@@ -5216,49 +5215,49 @@
         <v>-11602.572768806212</v>
       </c>
       <c r="E52" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>179058.10165151942</v>
       </c>
       <c r="F52" s="3">
+        <f t="shared" si="4"/>
+        <v>118115.52135505377</v>
+      </c>
+      <c r="G52" s="8">
         <f t="shared" si="5"/>
-        <v>111167.54951063888</v>
-      </c>
-      <c r="G52" s="8">
+        <v>60910.663023337067</v>
+      </c>
+      <c r="H52" s="8">
         <f t="shared" si="6"/>
-        <v>71510.871488517689</v>
-      </c>
-      <c r="H52" s="8">
+        <v>3175984.3326101815</v>
+      </c>
+      <c r="I52" s="8">
         <f t="shared" si="7"/>
-        <v>3218903.0398076149</v>
-      </c>
-      <c r="I52" s="8">
-        <f t="shared" si="8"/>
-        <v>3039844.9381560953</v>
+        <v>2996926.230958662</v>
       </c>
       <c r="J52" s="1">
         <f t="shared" si="3"/>
         <v>-807.2537033823545</v>
       </c>
       <c r="K52" s="9">
-        <f t="shared" si="9"/>
-        <v>2137.8374905892092</v>
+        <f t="shared" si="8"/>
+        <v>2271.4523337510341</v>
       </c>
       <c r="L52" s="2">
         <v>0</v>
       </c>
       <c r="M52" s="2">
-        <f t="shared" si="4"/>
-        <v>2320.5145537612425</v>
+        <f>-N52*tax_rate</f>
+        <v>-15227.665755834269</v>
       </c>
       <c r="N52" s="8">
-        <f t="shared" si="10"/>
-        <v>69190.356934756448</v>
+        <f t="shared" si="9"/>
+        <v>76138.328779171337</v>
       </c>
       <c r="O52" s="2"/>
       <c r="P52" s="2"/>
       <c r="Q52" s="2"/>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>26</v>
       </c>
@@ -5275,49 +5274,49 @@
         <v>-9919.8188314941872</v>
       </c>
       <c r="E53" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>147000.72790713116</v>
       </c>
       <c r="F53" s="3">
+        <f t="shared" si="4"/>
+        <v>125202.45263635699</v>
+      </c>
+      <c r="G53" s="8">
         <f t="shared" si="5"/>
-        <v>117837.60248127721</v>
-      </c>
-      <c r="G53" s="8">
+        <v>66580.208048379645</v>
+      </c>
+      <c r="H53" s="8">
         <f t="shared" si="6"/>
-        <v>77844.373671693611</v>
-      </c>
-      <c r="H53" s="8">
+        <v>3366543.3925667927</v>
+      </c>
+      <c r="I53" s="8">
         <f t="shared" si="7"/>
-        <v>3412037.2221960719</v>
-      </c>
-      <c r="I53" s="8">
-        <f t="shared" si="8"/>
-        <v>3265036.4942889409</v>
+        <v>3219542.6646596617</v>
       </c>
       <c r="J53" s="1">
         <f t="shared" si="3"/>
         <v>-807.2537033823545</v>
       </c>
       <c r="K53" s="9">
-        <f t="shared" si="9"/>
-        <v>2266.1077400245617</v>
+        <f t="shared" si="8"/>
+        <v>2407.739473776096</v>
       </c>
       <c r="L53" s="2">
         <v>0</v>
       </c>
       <c r="M53" s="2">
-        <f t="shared" si="4"/>
-        <v>1983.9637662988375</v>
+        <f>-N53*tax_rate</f>
+        <v>-16645.052012094911</v>
       </c>
       <c r="N53" s="8">
-        <f t="shared" si="10"/>
-        <v>75860.409905394772</v>
+        <f t="shared" si="9"/>
+        <v>83225.260060474553</v>
       </c>
       <c r="O53" s="2"/>
       <c r="P53" s="2"/>
       <c r="Q53" s="2"/>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>27</v>
       </c>
@@ -5334,49 +5333,49 @@
         <v>-8143.8403260550795</v>
       </c>
       <c r="E54" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>113167.37565730381</v>
       </c>
       <c r="F54" s="3">
+        <f t="shared" si="4"/>
+        <v>132714.5997945384</v>
+      </c>
+      <c r="G54" s="8">
         <f t="shared" si="5"/>
-        <v>124907.85863015385</v>
-      </c>
-      <c r="G54" s="8">
+        <v>72589.925774924777</v>
+      </c>
+      <c r="H54" s="8">
         <f t="shared" si="6"/>
-        <v>84559.434119482423</v>
-      </c>
-      <c r="H54" s="8">
+        <v>3568535.9961208003</v>
+      </c>
+      <c r="I54" s="8">
         <f t="shared" si="7"/>
-        <v>3616759.4555278365</v>
-      </c>
-      <c r="I54" s="8">
-        <f t="shared" si="8"/>
-        <v>3503592.0798705327</v>
+        <v>3455368.6204634965</v>
       </c>
       <c r="J54" s="1">
         <f t="shared" si="3"/>
         <v>-807.2537033823545</v>
       </c>
       <c r="K54" s="9">
-        <f t="shared" si="9"/>
-        <v>2402.0742044260355</v>
+        <f t="shared" si="8"/>
+        <v>2552.2038422026617</v>
       </c>
       <c r="L54" s="2">
         <v>0</v>
       </c>
       <c r="M54" s="2">
-        <f t="shared" si="4"/>
-        <v>1628.7680652110159</v>
+        <f>-N54*tax_rate</f>
+        <v>-18147.481443731194</v>
       </c>
       <c r="N54" s="8">
-        <f t="shared" si="10"/>
-        <v>82930.666054271409</v>
+        <f t="shared" si="9"/>
+        <v>90737.407218655964</v>
       </c>
       <c r="O54" s="2"/>
       <c r="P54" s="2"/>
       <c r="Q54" s="2"/>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>28</v>
       </c>
@@ -5393,49 +5392,49 @@
         <v>-6269.4726114146451</v>
       </c>
       <c r="E55" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>77459.655692836022</v>
       </c>
       <c r="F55" s="3">
+        <f t="shared" si="4"/>
+        <v>140677.47578221071</v>
+      </c>
+      <c r="G55" s="8">
         <f t="shared" si="5"/>
-        <v>132402.3301479631</v>
-      </c>
-      <c r="G55" s="8">
+        <v>78960.226565062621</v>
+      </c>
+      <c r="H55" s="8">
         <f t="shared" si="6"/>
-        <v>91679.032094363603</v>
-      </c>
-      <c r="H55" s="8">
+        <v>3782648.1558880485</v>
+      </c>
+      <c r="I55" s="8">
         <f t="shared" si="7"/>
-        <v>3833765.0228595068</v>
-      </c>
-      <c r="I55" s="8">
-        <f t="shared" si="8"/>
-        <v>3756305.367166671</v>
+        <v>3705188.5001952127</v>
       </c>
       <c r="J55" s="1">
         <f t="shared" si="3"/>
         <v>-807.2537033823545</v>
       </c>
       <c r="K55" s="9">
-        <f t="shared" si="9"/>
-        <v>2546.198656691598</v>
+        <f t="shared" si="8"/>
+        <v>2705.3360727348213</v>
       </c>
       <c r="L55" s="2">
         <v>0</v>
       </c>
       <c r="M55" s="2">
-        <f t="shared" si="4"/>
-        <v>1253.8945222829291</v>
+        <f>-N55*tax_rate</f>
+        <v>-19740.056641265655</v>
       </c>
       <c r="N55" s="8">
-        <f t="shared" si="10"/>
-        <v>90425.137572080668</v>
+        <f t="shared" si="9"/>
+        <v>98700.283206328269</v>
       </c>
       <c r="O55" s="2"/>
       <c r="P55" s="2"/>
       <c r="Q55" s="2"/>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>29</v>
       </c>
@@ -5452,49 +5451,49 @@
         <v>-4291.2649253831296</v>
       </c>
       <c r="E56" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>39773.728042336719</v>
       </c>
       <c r="F56" s="3">
+        <f t="shared" si="4"/>
+        <v>149118.12432914338</v>
+      </c>
+      <c r="G56" s="8">
         <f t="shared" si="5"/>
-        <v>140346.46995684091</v>
-      </c>
-      <c r="G56" s="8">
+        <v>85712.745402608751</v>
+      </c>
+      <c r="H56" s="8">
         <f t="shared" si="6"/>
-        <v>99227.530366035106</v>
-      </c>
-      <c r="H56" s="8">
+        <v>4009607.0452413317</v>
+      </c>
+      <c r="I56" s="8">
         <f t="shared" si="7"/>
-        <v>4063790.9242310775</v>
-      </c>
-      <c r="I56" s="8">
-        <f t="shared" si="8"/>
-        <v>4024017.1961887409</v>
+        <v>3969833.317198995</v>
       </c>
       <c r="J56" s="1">
         <f t="shared" si="3"/>
         <v>-807.2537033823545</v>
       </c>
       <c r="K56" s="9">
-        <f t="shared" si="9"/>
-        <v>2698.9705760930942</v>
+        <f t="shared" si="8"/>
+        <v>2867.6562370989109</v>
       </c>
       <c r="L56" s="2">
         <v>0</v>
       </c>
       <c r="M56" s="2">
-        <f t="shared" si="4"/>
-        <v>858.25298507662592</v>
+        <f>-N56*tax_rate</f>
+        <v>-21428.186350652191</v>
       </c>
       <c r="N56" s="8">
-        <f t="shared" si="10"/>
-        <v>98369.277380958476</v>
+        <f t="shared" si="9"/>
+        <v>107140.93175326094</v>
       </c>
       <c r="O56" s="2"/>
       <c r="P56" s="2"/>
       <c r="Q56" s="2"/>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>30</v>
       </c>
@@ -5511,49 +5510,49 @@
         <v>-2203.4645335454679</v>
       </c>
       <c r="E57" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>-2.4738255888223648E-10</v>
       </c>
       <c r="F57" s="3">
+        <f t="shared" si="4"/>
+        <v>158065.21178889199</v>
+      </c>
+      <c r="G57" s="8">
         <f t="shared" si="5"/>
-        <v>148767.25815425135</v>
-      </c>
-      <c r="G57" s="8">
+        <v>92870.415370407645</v>
+      </c>
+      <c r="H57" s="8">
         <f t="shared" si="6"/>
-        <v>107230.75848507801</v>
-      </c>
-      <c r="H57" s="8">
+        <v>4250183.4679558119</v>
+      </c>
+      <c r="I57" s="8">
         <f t="shared" si="7"/>
-        <v>4307618.3796849428</v>
-      </c>
-      <c r="I57" s="8">
-        <f t="shared" si="8"/>
-        <v>4307618.3796849428</v>
+        <v>4250183.4679558119</v>
       </c>
       <c r="J57" s="1">
         <f t="shared" si="3"/>
         <v>-807.2537033823545</v>
       </c>
       <c r="K57" s="9">
-        <f t="shared" si="9"/>
-        <v>2860.9088106586801</v>
+        <f t="shared" si="8"/>
+        <v>3039.7156113248457</v>
       </c>
       <c r="L57" s="2">
         <v>0</v>
       </c>
       <c r="M57" s="2">
-        <f t="shared" si="4"/>
-        <v>440.69290670909362</v>
+        <f>-N57*tax_rate</f>
+        <v>-23217.603842601911</v>
       </c>
       <c r="N57" s="8">
-        <f t="shared" si="10"/>
-        <v>106790.06557836891</v>
+        <f t="shared" si="9"/>
+        <v>116088.01921300955</v>
       </c>
       <c r="O57" s="2"/>
       <c r="P57" s="2"/>
       <c r="Q57" s="2"/>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="K58" s="1"/>
       <c r="L58" s="2"/>
       <c r="M58" s="2"/>
@@ -5561,7 +5560,7 @@
       <c r="P58" s="2"/>
       <c r="Q58" s="2"/>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="K59" s="1"/>
       <c r="L59" s="2"/>
       <c r="M59" s="2"/>
@@ -5569,7 +5568,7 @@
       <c r="P59" s="2"/>
       <c r="Q59" s="2"/>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="K60" s="1"/>
       <c r="L60" s="2"/>
       <c r="M60" s="2"/>
@@ -5577,7 +5576,7 @@
       <c r="P60" s="2"/>
       <c r="Q60" s="2"/>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="K61" s="1"/>
       <c r="L61" s="2"/>
       <c r="M61" s="2"/>
@@ -5585,7 +5584,7 @@
       <c r="P61" s="2"/>
       <c r="Q61" s="2"/>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="K62" s="1"/>
       <c r="Q62" s="2"/>
     </row>

</xml_diff>